<commit_message>
updated tasks to gantt chart
</commit_message>
<xml_diff>
--- a/docs/planningdocuments/gannt/GanttChart_POS_8.xlsx
+++ b/docs/planningdocuments/gannt/GanttChart_POS_8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CPS353-POS\docs\planningdocuments\gannt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/CPS353-POS/docs/planningdocuments/gannt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3AEF26C-1734-4E76-AB11-2F993C5B3D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB733159-A4B2-E44F-A1FB-8584B1BCD3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="142">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -536,6 +536,12 @@
   </si>
   <si>
     <t>W14 11/28/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Data Validation to Admin Invetory </t>
+  </si>
+  <si>
+    <t>Get Admin Page Connected to DB</t>
   </si>
 </sst>
 </file>
@@ -1539,27 +1545,13 @@
     <xf numFmtId="0" fontId="27" fillId="28" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1574,9 +1566,14 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1587,13 +1584,22 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1912,26 +1918,26 @@
     <tabColor rgb="FF3D85C6"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BZ112"/>
+  <dimension ref="A1:BZ115"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112:XFD112"/>
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="62" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="33" width="3.44140625" hidden="1" customWidth="1"/>
-    <col min="34" max="78" width="3.44140625" customWidth="1"/>
+    <col min="9" max="33" width="3.5" hidden="1" customWidth="1"/>
+    <col min="34" max="78" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2011,40 +2017,40 @@
       <c r="BY1" s="1"/>
       <c r="BZ1" s="1"/>
     </row>
-    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
+      <c r="C2" s="157"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="157"/>
+      <c r="G2" s="157"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="165"/>
-      <c r="M2" s="165"/>
-      <c r="N2" s="165"/>
-      <c r="O2" s="167"/>
-      <c r="P2" s="165"/>
-      <c r="Q2" s="165"/>
-      <c r="R2" s="165"/>
-      <c r="S2" s="165"/>
-      <c r="T2" s="165"/>
-      <c r="U2" s="165"/>
-      <c r="V2" s="165"/>
-      <c r="W2" s="165"/>
-      <c r="X2" s="165"/>
-      <c r="Y2" s="165"/>
-      <c r="Z2" s="165"/>
-      <c r="AA2" s="165"/>
-      <c r="AB2" s="165"/>
-      <c r="AC2" s="165"/>
-      <c r="AD2" s="165"/>
-      <c r="AE2" s="165"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="157"/>
+      <c r="K2" s="157"/>
+      <c r="L2" s="157"/>
+      <c r="M2" s="157"/>
+      <c r="N2" s="157"/>
+      <c r="O2" s="159"/>
+      <c r="P2" s="157"/>
+      <c r="Q2" s="157"/>
+      <c r="R2" s="157"/>
+      <c r="S2" s="157"/>
+      <c r="T2" s="157"/>
+      <c r="U2" s="157"/>
+      <c r="V2" s="157"/>
+      <c r="W2" s="157"/>
+      <c r="X2" s="157"/>
+      <c r="Y2" s="157"/>
+      <c r="Z2" s="157"/>
+      <c r="AA2" s="157"/>
+      <c r="AB2" s="157"/>
+      <c r="AC2" s="157"/>
+      <c r="AD2" s="157"/>
+      <c r="AE2" s="157"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -2093,7 +2099,7 @@
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
     </row>
-    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -2173,43 +2179,43 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
     </row>
-    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="158"/>
-      <c r="D4" s="168" t="s">
+      <c r="C4" s="161"/>
+      <c r="D4" s="162" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="157" t="s">
+      <c r="I4" s="160" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="158"/>
-      <c r="K4" s="158"/>
-      <c r="L4" s="158"/>
-      <c r="M4" s="158"/>
-      <c r="N4" s="158"/>
-      <c r="O4" s="158"/>
-      <c r="P4" s="169" t="s">
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
+      <c r="L4" s="161"/>
+      <c r="M4" s="161"/>
+      <c r="N4" s="161"/>
+      <c r="O4" s="161"/>
+      <c r="P4" s="164" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="160"/>
-      <c r="R4" s="160"/>
-      <c r="S4" s="160"/>
-      <c r="T4" s="160"/>
-      <c r="U4" s="160"/>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="160"/>
-      <c r="Z4" s="160"/>
-      <c r="AA4" s="160"/>
-      <c r="AB4" s="160"/>
+      <c r="Q4" s="163"/>
+      <c r="R4" s="163"/>
+      <c r="S4" s="163"/>
+      <c r="T4" s="163"/>
+      <c r="U4" s="163"/>
+      <c r="V4" s="163"/>
+      <c r="W4" s="163"/>
+      <c r="X4" s="163"/>
+      <c r="Y4" s="163"/>
+      <c r="Z4" s="163"/>
+      <c r="AA4" s="163"/>
+      <c r="AB4" s="163"/>
       <c r="AC4" s="17"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
@@ -2261,42 +2267,42 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="157" t="s">
+      <c r="B5" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="158"/>
-      <c r="D5" s="159" t="s">
+      <c r="C5" s="161"/>
+      <c r="D5" s="174" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="157" t="s">
+      <c r="I5" s="160" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="158"/>
-      <c r="K5" s="158"/>
-      <c r="L5" s="158"/>
-      <c r="M5" s="158"/>
-      <c r="N5" s="158"/>
-      <c r="O5" s="158"/>
-      <c r="P5" s="161">
+      <c r="J5" s="161"/>
+      <c r="K5" s="161"/>
+      <c r="L5" s="161"/>
+      <c r="M5" s="161"/>
+      <c r="N5" s="161"/>
+      <c r="O5" s="161"/>
+      <c r="P5" s="175">
         <v>44858</v>
       </c>
-      <c r="Q5" s="160"/>
-      <c r="R5" s="160"/>
-      <c r="S5" s="160"/>
-      <c r="T5" s="160"/>
-      <c r="U5" s="160"/>
-      <c r="V5" s="160"/>
-      <c r="W5" s="160"/>
-      <c r="X5" s="160"/>
-      <c r="Y5" s="160"/>
-      <c r="Z5" s="160"/>
-      <c r="AA5" s="160"/>
+      <c r="Q5" s="163"/>
+      <c r="R5" s="163"/>
+      <c r="S5" s="163"/>
+      <c r="T5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
+      <c r="X5" s="163"/>
+      <c r="Y5" s="163"/>
+      <c r="Z5" s="163"/>
+      <c r="AA5" s="163"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="1"/>
@@ -2349,7 +2355,7 @@
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
     </row>
-    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="21"/>
       <c r="B6" s="48" t="s">
         <v>44</v>
@@ -2433,7 +2439,7 @@
       <c r="BY6" s="21"/>
       <c r="BZ6" s="21"/>
     </row>
-    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="21"/>
       <c r="B7" s="22" t="s">
         <v>45</v>
@@ -2517,7 +2523,7 @@
       <c r="BY7" s="21"/>
       <c r="BZ7" s="21"/>
     </row>
-    <row r="8" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="21"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
@@ -2597,209 +2603,209 @@
       <c r="BY8" s="21"/>
       <c r="BZ8" s="21"/>
     </row>
-    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="24"/>
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="162" t="s">
+      <c r="C9" s="154" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="162" t="s">
+      <c r="D9" s="154" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="162" t="s">
+      <c r="E9" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="162" t="s">
+      <c r="F9" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="162" t="s">
+      <c r="G9" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="170" t="s">
+      <c r="H9" s="165" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="172"/>
-      <c r="J9" s="152"/>
-      <c r="K9" s="152"/>
-      <c r="L9" s="152"/>
-      <c r="M9" s="152"/>
-      <c r="N9" s="152"/>
-      <c r="O9" s="152"/>
-      <c r="P9" s="152"/>
-      <c r="Q9" s="152"/>
-      <c r="R9" s="152"/>
-      <c r="S9" s="152"/>
-      <c r="T9" s="152"/>
-      <c r="U9" s="152"/>
-      <c r="V9" s="152"/>
-      <c r="W9" s="152"/>
-      <c r="X9" s="151"/>
-      <c r="Y9" s="152"/>
-      <c r="Z9" s="152"/>
-      <c r="AA9" s="152"/>
-      <c r="AB9" s="152"/>
-      <c r="AC9" s="152"/>
-      <c r="AD9" s="152"/>
-      <c r="AE9" s="152"/>
-      <c r="AF9" s="152"/>
-      <c r="AG9" s="152"/>
-      <c r="AH9" s="152"/>
-      <c r="AI9" s="152"/>
-      <c r="AJ9" s="152"/>
-      <c r="AK9" s="152"/>
-      <c r="AL9" s="152"/>
-      <c r="AM9" s="151"/>
-      <c r="AN9" s="152"/>
-      <c r="AO9" s="152"/>
-      <c r="AP9" s="152"/>
-      <c r="AQ9" s="152"/>
-      <c r="AR9" s="152"/>
-      <c r="AS9" s="152"/>
-      <c r="AT9" s="152"/>
-      <c r="AU9" s="152"/>
-      <c r="AV9" s="152"/>
-      <c r="AW9" s="152"/>
-      <c r="AX9" s="152"/>
-      <c r="AY9" s="152"/>
-      <c r="AZ9" s="152"/>
-      <c r="BA9" s="152"/>
-      <c r="BB9" s="151"/>
-      <c r="BC9" s="152"/>
-      <c r="BD9" s="152"/>
-      <c r="BE9" s="152"/>
-      <c r="BF9" s="152"/>
-      <c r="BG9" s="152"/>
-      <c r="BH9" s="152"/>
-      <c r="BI9" s="152"/>
-      <c r="BJ9" s="152"/>
-      <c r="BK9" s="152"/>
-      <c r="BL9" s="152"/>
-      <c r="BM9" s="152"/>
-      <c r="BN9" s="152"/>
-      <c r="BO9" s="152"/>
-      <c r="BP9" s="152"/>
-      <c r="BQ9" s="152"/>
-      <c r="BR9" s="152"/>
-      <c r="BS9" s="152"/>
-      <c r="BT9" s="152"/>
-      <c r="BU9" s="152"/>
-      <c r="BV9" s="152"/>
-      <c r="BW9" s="152"/>
-      <c r="BX9" s="152"/>
-      <c r="BY9" s="152"/>
-      <c r="BZ9" s="153"/>
+      <c r="I9" s="167"/>
+      <c r="J9" s="168"/>
+      <c r="K9" s="168"/>
+      <c r="L9" s="168"/>
+      <c r="M9" s="168"/>
+      <c r="N9" s="168"/>
+      <c r="O9" s="168"/>
+      <c r="P9" s="168"/>
+      <c r="Q9" s="168"/>
+      <c r="R9" s="168"/>
+      <c r="S9" s="168"/>
+      <c r="T9" s="168"/>
+      <c r="U9" s="168"/>
+      <c r="V9" s="168"/>
+      <c r="W9" s="168"/>
+      <c r="X9" s="169"/>
+      <c r="Y9" s="168"/>
+      <c r="Z9" s="168"/>
+      <c r="AA9" s="168"/>
+      <c r="AB9" s="168"/>
+      <c r="AC9" s="168"/>
+      <c r="AD9" s="168"/>
+      <c r="AE9" s="168"/>
+      <c r="AF9" s="168"/>
+      <c r="AG9" s="168"/>
+      <c r="AH9" s="168"/>
+      <c r="AI9" s="168"/>
+      <c r="AJ9" s="168"/>
+      <c r="AK9" s="168"/>
+      <c r="AL9" s="168"/>
+      <c r="AM9" s="169"/>
+      <c r="AN9" s="168"/>
+      <c r="AO9" s="168"/>
+      <c r="AP9" s="168"/>
+      <c r="AQ9" s="168"/>
+      <c r="AR9" s="168"/>
+      <c r="AS9" s="168"/>
+      <c r="AT9" s="168"/>
+      <c r="AU9" s="168"/>
+      <c r="AV9" s="168"/>
+      <c r="AW9" s="168"/>
+      <c r="AX9" s="168"/>
+      <c r="AY9" s="168"/>
+      <c r="AZ9" s="168"/>
+      <c r="BA9" s="168"/>
+      <c r="BB9" s="169"/>
+      <c r="BC9" s="168"/>
+      <c r="BD9" s="168"/>
+      <c r="BE9" s="168"/>
+      <c r="BF9" s="168"/>
+      <c r="BG9" s="168"/>
+      <c r="BH9" s="168"/>
+      <c r="BI9" s="168"/>
+      <c r="BJ9" s="168"/>
+      <c r="BK9" s="168"/>
+      <c r="BL9" s="168"/>
+      <c r="BM9" s="168"/>
+      <c r="BN9" s="168"/>
+      <c r="BO9" s="168"/>
+      <c r="BP9" s="168"/>
+      <c r="BQ9" s="168"/>
+      <c r="BR9" s="168"/>
+      <c r="BS9" s="168"/>
+      <c r="BT9" s="168"/>
+      <c r="BU9" s="168"/>
+      <c r="BV9" s="168"/>
+      <c r="BW9" s="168"/>
+      <c r="BX9" s="168"/>
+      <c r="BY9" s="168"/>
+      <c r="BZ9" s="173"/>
     </row>
-    <row r="10" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="25"/>
-      <c r="B10" s="163"/>
-      <c r="C10" s="163"/>
-      <c r="D10" s="163"/>
-      <c r="E10" s="163"/>
-      <c r="F10" s="163"/>
-      <c r="G10" s="163"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="154" t="s">
+      <c r="B10" s="155"/>
+      <c r="C10" s="155"/>
+      <c r="D10" s="155"/>
+      <c r="E10" s="155"/>
+      <c r="F10" s="155"/>
+      <c r="G10" s="155"/>
+      <c r="H10" s="166"/>
+      <c r="I10" s="170" t="s">
         <v>95</v>
       </c>
-      <c r="J10" s="155"/>
-      <c r="K10" s="155"/>
-      <c r="L10" s="155"/>
-      <c r="M10" s="156"/>
-      <c r="N10" s="154" t="s">
+      <c r="J10" s="171"/>
+      <c r="K10" s="171"/>
+      <c r="L10" s="171"/>
+      <c r="M10" s="172"/>
+      <c r="N10" s="170" t="s">
         <v>96</v>
       </c>
-      <c r="O10" s="155"/>
-      <c r="P10" s="155"/>
-      <c r="Q10" s="155"/>
-      <c r="R10" s="156"/>
-      <c r="S10" s="154" t="s">
+      <c r="O10" s="171"/>
+      <c r="P10" s="171"/>
+      <c r="Q10" s="171"/>
+      <c r="R10" s="172"/>
+      <c r="S10" s="170" t="s">
         <v>97</v>
       </c>
-      <c r="T10" s="155"/>
-      <c r="U10" s="155"/>
-      <c r="V10" s="155"/>
-      <c r="W10" s="156"/>
-      <c r="X10" s="154" t="s">
+      <c r="T10" s="171"/>
+      <c r="U10" s="171"/>
+      <c r="V10" s="171"/>
+      <c r="W10" s="172"/>
+      <c r="X10" s="170" t="s">
         <v>103</v>
       </c>
-      <c r="Y10" s="155"/>
-      <c r="Z10" s="155"/>
-      <c r="AA10" s="155"/>
-      <c r="AB10" s="156"/>
-      <c r="AC10" s="154" t="s">
+      <c r="Y10" s="171"/>
+      <c r="Z10" s="171"/>
+      <c r="AA10" s="171"/>
+      <c r="AB10" s="172"/>
+      <c r="AC10" s="170" t="s">
         <v>104</v>
       </c>
-      <c r="AD10" s="155"/>
-      <c r="AE10" s="155"/>
-      <c r="AF10" s="155"/>
-      <c r="AG10" s="156"/>
-      <c r="AH10" s="154" t="s">
+      <c r="AD10" s="171"/>
+      <c r="AE10" s="171"/>
+      <c r="AF10" s="171"/>
+      <c r="AG10" s="172"/>
+      <c r="AH10" s="170" t="s">
         <v>81</v>
       </c>
-      <c r="AI10" s="155"/>
-      <c r="AJ10" s="155"/>
-      <c r="AK10" s="155"/>
-      <c r="AL10" s="156"/>
-      <c r="AM10" s="154" t="s">
+      <c r="AI10" s="171"/>
+      <c r="AJ10" s="171"/>
+      <c r="AK10" s="171"/>
+      <c r="AL10" s="172"/>
+      <c r="AM10" s="170" t="s">
         <v>133</v>
       </c>
-      <c r="AN10" s="155"/>
-      <c r="AO10" s="155"/>
-      <c r="AP10" s="155"/>
-      <c r="AQ10" s="156"/>
-      <c r="AR10" s="154" t="s">
+      <c r="AN10" s="171"/>
+      <c r="AO10" s="171"/>
+      <c r="AP10" s="171"/>
+      <c r="AQ10" s="172"/>
+      <c r="AR10" s="170" t="s">
         <v>134</v>
       </c>
-      <c r="AS10" s="155"/>
-      <c r="AT10" s="155"/>
-      <c r="AU10" s="155"/>
-      <c r="AV10" s="156"/>
-      <c r="AW10" s="154" t="s">
+      <c r="AS10" s="171"/>
+      <c r="AT10" s="171"/>
+      <c r="AU10" s="171"/>
+      <c r="AV10" s="172"/>
+      <c r="AW10" s="170" t="s">
         <v>105</v>
       </c>
-      <c r="AX10" s="155"/>
-      <c r="AY10" s="155"/>
-      <c r="AZ10" s="155"/>
-      <c r="BA10" s="156"/>
-      <c r="BB10" s="154" t="s">
+      <c r="AX10" s="171"/>
+      <c r="AY10" s="171"/>
+      <c r="AZ10" s="171"/>
+      <c r="BA10" s="172"/>
+      <c r="BB10" s="170" t="s">
         <v>135</v>
       </c>
-      <c r="BC10" s="155"/>
-      <c r="BD10" s="155"/>
-      <c r="BE10" s="155"/>
-      <c r="BF10" s="156"/>
-      <c r="BG10" s="154" t="s">
+      <c r="BC10" s="171"/>
+      <c r="BD10" s="171"/>
+      <c r="BE10" s="171"/>
+      <c r="BF10" s="172"/>
+      <c r="BG10" s="170" t="s">
         <v>136</v>
       </c>
-      <c r="BH10" s="155"/>
-      <c r="BI10" s="155"/>
-      <c r="BJ10" s="155"/>
-      <c r="BK10" s="156"/>
-      <c r="BL10" s="154" t="s">
+      <c r="BH10" s="171"/>
+      <c r="BI10" s="171"/>
+      <c r="BJ10" s="171"/>
+      <c r="BK10" s="172"/>
+      <c r="BL10" s="170" t="s">
         <v>137</v>
       </c>
-      <c r="BM10" s="155"/>
-      <c r="BN10" s="155"/>
-      <c r="BO10" s="155"/>
-      <c r="BP10" s="156"/>
-      <c r="BQ10" s="154" t="s">
+      <c r="BM10" s="171"/>
+      <c r="BN10" s="171"/>
+      <c r="BO10" s="171"/>
+      <c r="BP10" s="172"/>
+      <c r="BQ10" s="170" t="s">
         <v>138</v>
       </c>
-      <c r="BR10" s="155"/>
-      <c r="BS10" s="155"/>
-      <c r="BT10" s="155"/>
-      <c r="BU10" s="156"/>
-      <c r="BV10" s="154" t="s">
+      <c r="BR10" s="171"/>
+      <c r="BS10" s="171"/>
+      <c r="BT10" s="171"/>
+      <c r="BU10" s="172"/>
+      <c r="BV10" s="170" t="s">
         <v>139</v>
       </c>
-      <c r="BW10" s="155"/>
-      <c r="BX10" s="155"/>
-      <c r="BY10" s="155"/>
-      <c r="BZ10" s="156"/>
+      <c r="BW10" s="171"/>
+      <c r="BX10" s="171"/>
+      <c r="BY10" s="171"/>
+      <c r="BZ10" s="172"/>
     </row>
-    <row r="11" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="21"/>
       <c r="B11" s="26">
         <v>1</v>
@@ -3023,7 +3029,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A12" s="32"/>
       <c r="B12" s="33">
         <v>1.1000000000000001</v>
@@ -3118,7 +3124,7 @@
       <c r="BY12" s="38"/>
       <c r="BZ12" s="38"/>
     </row>
-    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A13" s="32"/>
       <c r="B13" s="33" t="s">
         <v>12</v>
@@ -3213,7 +3219,7 @@
       <c r="BY13" s="38"/>
       <c r="BZ13" s="38"/>
     </row>
-    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A14" s="32"/>
       <c r="B14" s="33">
         <v>1.2</v>
@@ -3308,7 +3314,7 @@
       <c r="BY14" s="38"/>
       <c r="BZ14" s="38"/>
     </row>
-    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A15" s="32"/>
       <c r="B15" s="33">
         <v>1.3</v>
@@ -3403,7 +3409,7 @@
       <c r="BY15" s="38"/>
       <c r="BZ15" s="38"/>
     </row>
-    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A16" s="32"/>
       <c r="B16" s="33">
         <v>1.4</v>
@@ -3498,7 +3504,7 @@
       <c r="BY16" s="38"/>
       <c r="BZ16" s="38"/>
     </row>
-    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A17" s="32"/>
       <c r="B17" s="33">
         <v>1.5</v>
@@ -3593,7 +3599,7 @@
       <c r="BY17" s="38"/>
       <c r="BZ17" s="38"/>
     </row>
-    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A18" s="32"/>
       <c r="B18" s="33">
         <v>1.6</v>
@@ -3688,7 +3694,7 @@
       <c r="BY18" s="38"/>
       <c r="BZ18" s="38"/>
     </row>
-    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A19" s="32"/>
       <c r="B19" s="33">
         <v>1.7</v>
@@ -3783,7 +3789,7 @@
       <c r="BY19" s="38"/>
       <c r="BZ19" s="38"/>
     </row>
-    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A20" s="32"/>
       <c r="B20" s="33"/>
       <c r="C20" s="34"/>
@@ -3863,7 +3869,7 @@
       <c r="BY20" s="38"/>
       <c r="BZ20" s="38"/>
     </row>
-    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A21" s="32"/>
       <c r="B21" s="33"/>
       <c r="C21" s="34"/>
@@ -3943,7 +3949,7 @@
       <c r="BY21" s="38"/>
       <c r="BZ21" s="38"/>
     </row>
-    <row r="22" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="21"/>
       <c r="B22" s="26">
         <v>2</v>
@@ -4027,7 +4033,7 @@
       <c r="BY22" s="29"/>
       <c r="BZ22" s="29"/>
     </row>
-    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A23" s="32"/>
       <c r="B23" s="33">
         <v>2.1</v>
@@ -4117,7 +4123,7 @@
       <c r="BY23" s="38"/>
       <c r="BZ23" s="38"/>
     </row>
-    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A24" s="32"/>
       <c r="B24" s="33">
         <v>2.2000000000000002</v>
@@ -4208,7 +4214,7 @@
       <c r="BY24" s="38"/>
       <c r="BZ24" s="38"/>
     </row>
-    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A25" s="32"/>
       <c r="B25" s="33">
         <v>2.2999999999999998</v>
@@ -4299,7 +4305,7 @@
       <c r="BY25" s="38"/>
       <c r="BZ25" s="38"/>
     </row>
-    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A26" s="32"/>
       <c r="B26" s="33" t="s">
         <v>13</v>
@@ -4389,7 +4395,7 @@
       <c r="BY26" s="38"/>
       <c r="BZ26" s="38"/>
     </row>
-    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A27" s="32"/>
       <c r="B27" s="33">
         <v>2.4</v>
@@ -4480,7 +4486,7 @@
       <c r="BY27" s="38"/>
       <c r="BZ27" s="38"/>
     </row>
-    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A28" s="32"/>
       <c r="B28" s="33">
         <v>2.5</v>
@@ -4571,7 +4577,7 @@
       <c r="BY28" s="38"/>
       <c r="BZ28" s="38"/>
     </row>
-    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A29" s="32"/>
       <c r="B29" s="33">
         <v>2.6</v>
@@ -4661,7 +4667,7 @@
       <c r="BY29" s="38"/>
       <c r="BZ29" s="38"/>
     </row>
-    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A30" s="32"/>
       <c r="B30" s="33">
         <v>2.7</v>
@@ -4752,7 +4758,7 @@
       <c r="BY30" s="38"/>
       <c r="BZ30" s="38"/>
     </row>
-    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A31" s="32"/>
       <c r="B31" s="33">
         <v>2.8</v>
@@ -4843,7 +4849,7 @@
       <c r="BY31" s="38"/>
       <c r="BZ31" s="38"/>
     </row>
-    <row r="32" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A32" s="32"/>
       <c r="B32" s="33">
         <v>2.9</v>
@@ -4933,7 +4939,7 @@
       <c r="BY32" s="38"/>
       <c r="BZ32" s="38"/>
     </row>
-    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A33" s="32"/>
       <c r="B33" s="46">
         <v>2.1</v>
@@ -5023,7 +5029,7 @@
       <c r="BY33" s="38"/>
       <c r="BZ33" s="38"/>
     </row>
-    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A34" s="32"/>
       <c r="B34" s="46">
         <v>2.11</v>
@@ -5105,7 +5111,7 @@
       <c r="BY34" s="38"/>
       <c r="BZ34" s="38"/>
     </row>
-    <row r="35" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="21"/>
       <c r="B35" s="26">
         <v>3</v>
@@ -5189,7 +5195,7 @@
       <c r="BY35" s="29"/>
       <c r="BZ35" s="29"/>
     </row>
-    <row r="36" spans="1:78" s="75" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:78" s="75" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="78"/>
       <c r="B36" s="79"/>
       <c r="C36" s="80" t="s">
@@ -5271,7 +5277,7 @@
       <c r="BY36" s="82"/>
       <c r="BZ36" s="82"/>
     </row>
-    <row r="37" spans="1:78" s="105" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:78" s="105" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="134"/>
       <c r="B37" s="135"/>
       <c r="C37" s="136" t="s">
@@ -5353,7 +5359,7 @@
       <c r="BY37" s="138"/>
       <c r="BZ37" s="138"/>
     </row>
-    <row r="38" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="21"/>
       <c r="B38" s="85"/>
       <c r="C38" s="120" t="s">
@@ -5435,7 +5441,7 @@
       <c r="BY38" s="88"/>
       <c r="BZ38" s="88"/>
     </row>
-    <row r="39" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="21"/>
       <c r="B39" s="85"/>
       <c r="C39" s="120" t="s">
@@ -5478,12 +5484,12 @@
       <c r="AL39" s="88"/>
       <c r="AM39" s="88"/>
       <c r="AN39" s="88"/>
-      <c r="AO39" s="174"/>
-      <c r="AP39" s="174"/>
-      <c r="AQ39" s="174"/>
-      <c r="AR39" s="174"/>
-      <c r="AS39" s="174"/>
-      <c r="AT39" s="175"/>
+      <c r="AO39" s="152"/>
+      <c r="AP39" s="152"/>
+      <c r="AQ39" s="152"/>
+      <c r="AR39" s="152"/>
+      <c r="AS39" s="152"/>
+      <c r="AT39" s="153"/>
       <c r="AU39" s="122"/>
       <c r="AV39" s="88"/>
       <c r="AW39" s="88"/>
@@ -5517,7 +5523,7 @@
       <c r="BY39" s="88"/>
       <c r="BZ39" s="88"/>
     </row>
-    <row r="40" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="21"/>
       <c r="B40" s="85"/>
       <c r="C40" s="120" t="s">
@@ -5599,7 +5605,7 @@
       <c r="BY40" s="88"/>
       <c r="BZ40" s="88"/>
     </row>
-    <row r="41" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="21"/>
       <c r="B41" s="85"/>
       <c r="C41" s="120" t="s">
@@ -5681,7 +5687,7 @@
       <c r="BY41" s="88"/>
       <c r="BZ41" s="88"/>
     </row>
-    <row r="42" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="21"/>
       <c r="B42" s="85"/>
       <c r="C42" s="120" t="s">
@@ -5763,7 +5769,7 @@
       <c r="BY42" s="88"/>
       <c r="BZ42" s="88"/>
     </row>
-    <row r="43" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="21"/>
       <c r="B43" s="85"/>
       <c r="C43" s="120"/>
@@ -5843,7 +5849,7 @@
       <c r="BY43" s="88"/>
       <c r="BZ43" s="88"/>
     </row>
-    <row r="44" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="21"/>
       <c r="B44" s="85"/>
       <c r="C44" s="120"/>
@@ -5923,7 +5929,7 @@
       <c r="BY44" s="88"/>
       <c r="BZ44" s="88"/>
     </row>
-    <row r="45" spans="1:78" s="105" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:78" s="105" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="134"/>
       <c r="B45" s="142"/>
       <c r="C45" s="143" t="s">
@@ -6005,7 +6011,7 @@
       <c r="BY45" s="141"/>
       <c r="BZ45" s="141"/>
     </row>
-    <row r="46" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="21"/>
       <c r="B46" s="85"/>
       <c r="C46" s="120" t="s">
@@ -6087,7 +6093,7 @@
       <c r="BY46" s="88"/>
       <c r="BZ46" s="88"/>
     </row>
-    <row r="47" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="21"/>
       <c r="B47" s="85"/>
       <c r="C47" s="120" t="s">
@@ -6169,7 +6175,7 @@
       <c r="BY47" s="88"/>
       <c r="BZ47" s="88"/>
     </row>
-    <row r="48" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="21"/>
       <c r="B48" s="85"/>
       <c r="C48" s="120" t="s">
@@ -6251,7 +6257,7 @@
       <c r="BY48" s="88"/>
       <c r="BZ48" s="88"/>
     </row>
-    <row r="49" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="21"/>
       <c r="B49" s="85"/>
       <c r="C49" s="120" t="s">
@@ -6333,7 +6339,7 @@
       <c r="BY49" s="88"/>
       <c r="BZ49" s="88"/>
     </row>
-    <row r="50" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="21"/>
       <c r="B50" s="85"/>
       <c r="C50" s="86"/>
@@ -6413,7 +6419,7 @@
       <c r="BY50" s="88"/>
       <c r="BZ50" s="88"/>
     </row>
-    <row r="51" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="21"/>
       <c r="B51" s="85"/>
       <c r="C51" s="86"/>
@@ -6493,7 +6499,7 @@
       <c r="BY51" s="88"/>
       <c r="BZ51" s="88"/>
     </row>
-    <row r="52" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A52" s="72"/>
       <c r="B52" s="73"/>
       <c r="C52" s="76" t="s">
@@ -6575,7 +6581,7 @@
       <c r="BY52" s="67"/>
       <c r="BZ52" s="67"/>
     </row>
-    <row r="53" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A53" s="32"/>
       <c r="B53" s="53"/>
       <c r="C53" s="56" t="s">
@@ -6657,7 +6663,7 @@
       <c r="BY53" s="38"/>
       <c r="BZ53" s="38"/>
     </row>
-    <row r="54" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A54" s="32"/>
       <c r="B54" s="53"/>
       <c r="C54" s="56" t="s">
@@ -6739,7 +6745,7 @@
       <c r="BY54" s="38"/>
       <c r="BZ54" s="38"/>
     </row>
-    <row r="55" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A55" s="32"/>
       <c r="B55" s="53"/>
       <c r="C55" s="56" t="s">
@@ -6821,7 +6827,7 @@
       <c r="BY55" s="38"/>
       <c r="BZ55" s="38"/>
     </row>
-    <row r="56" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A56" s="32"/>
       <c r="B56" s="53"/>
       <c r="C56" s="56" t="s">
@@ -6903,7 +6909,7 @@
       <c r="BY56" s="38"/>
       <c r="BZ56" s="38"/>
     </row>
-    <row r="57" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A57" s="32"/>
       <c r="B57" s="53"/>
       <c r="C57" s="56" t="s">
@@ -6985,7 +6991,7 @@
       <c r="BY57" s="38"/>
       <c r="BZ57" s="38"/>
     </row>
-    <row r="58" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A58" s="32"/>
       <c r="B58" s="53"/>
       <c r="C58" s="56" t="s">
@@ -7026,11 +7032,11 @@
       <c r="AJ58" s="38"/>
       <c r="AK58" s="38"/>
       <c r="AL58" s="38"/>
-      <c r="AM58" s="175"/>
-      <c r="AN58" s="173"/>
-      <c r="AO58" s="173"/>
-      <c r="AP58" s="173"/>
-      <c r="AQ58" s="173"/>
+      <c r="AM58" s="153"/>
+      <c r="AN58" s="151"/>
+      <c r="AO58" s="151"/>
+      <c r="AP58" s="151"/>
+      <c r="AQ58" s="151"/>
       <c r="AR58" s="150"/>
       <c r="AS58" s="150"/>
       <c r="AT58" s="150"/>
@@ -7067,7 +7073,7 @@
       <c r="BY58" s="38"/>
       <c r="BZ58" s="38"/>
     </row>
-    <row r="59" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A59" s="32"/>
       <c r="B59" s="53"/>
       <c r="C59" s="56" t="s">
@@ -7149,7 +7155,7 @@
       <c r="BY59" s="38"/>
       <c r="BZ59" s="38"/>
     </row>
-    <row r="60" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A60" s="32"/>
       <c r="B60" s="53"/>
       <c r="C60" s="56" t="s">
@@ -7231,7 +7237,7 @@
       <c r="BY60" s="38"/>
       <c r="BZ60" s="38"/>
     </row>
-    <row r="61" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A61" s="32"/>
       <c r="B61" s="53"/>
       <c r="C61" s="56" t="s">
@@ -7313,7 +7319,7 @@
       <c r="BY61" s="38"/>
       <c r="BZ61" s="38"/>
     </row>
-    <row r="62" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A62" s="32"/>
       <c r="B62" s="53"/>
       <c r="C62" s="56" t="s">
@@ -7395,7 +7401,7 @@
       <c r="BY62" s="38"/>
       <c r="BZ62" s="38"/>
     </row>
-    <row r="63" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A63" s="32"/>
       <c r="B63" s="53"/>
       <c r="C63" s="56" t="s">
@@ -7477,7 +7483,7 @@
       <c r="BY63" s="38"/>
       <c r="BZ63" s="38"/>
     </row>
-    <row r="64" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A64" s="32"/>
       <c r="B64" s="53"/>
       <c r="C64" s="56" t="s">
@@ -7559,7 +7565,7 @@
       <c r="BY64" s="38"/>
       <c r="BZ64" s="38"/>
     </row>
-    <row r="65" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A65" s="32"/>
       <c r="B65" s="53"/>
       <c r="C65" s="56" t="s">
@@ -7600,11 +7606,11 @@
       <c r="AJ65" s="38"/>
       <c r="AK65" s="38"/>
       <c r="AL65" s="38"/>
-      <c r="AM65" s="173"/>
-      <c r="AN65" s="173"/>
-      <c r="AO65" s="173"/>
-      <c r="AP65" s="173"/>
-      <c r="AQ65" s="173"/>
+      <c r="AM65" s="151"/>
+      <c r="AN65" s="151"/>
+      <c r="AO65" s="151"/>
+      <c r="AP65" s="151"/>
+      <c r="AQ65" s="151"/>
       <c r="AR65" s="40"/>
       <c r="AS65" s="40"/>
       <c r="AT65" s="124"/>
@@ -7641,7 +7647,7 @@
       <c r="BY65" s="38"/>
       <c r="BZ65" s="38"/>
     </row>
-    <row r="66" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A66" s="32"/>
       <c r="B66" s="53"/>
       <c r="C66" s="56"/>
@@ -7721,7 +7727,7 @@
       <c r="BY66" s="38"/>
       <c r="BZ66" s="38"/>
     </row>
-    <row r="67" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A67" s="32"/>
       <c r="B67" s="53"/>
       <c r="C67" s="56"/>
@@ -7801,7 +7807,7 @@
       <c r="BY67" s="38"/>
       <c r="BZ67" s="38"/>
     </row>
-    <row r="68" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A68" s="32"/>
       <c r="B68" s="59"/>
       <c r="C68" s="60" t="s">
@@ -7883,7 +7889,7 @@
       <c r="BY68" s="67"/>
       <c r="BZ68" s="67"/>
     </row>
-    <row r="69" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A69" s="32"/>
       <c r="B69" s="53"/>
       <c r="C69" s="56" t="s">
@@ -7965,7 +7971,7 @@
       <c r="BY69" s="38"/>
       <c r="BZ69" s="38"/>
     </row>
-    <row r="70" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A70" s="32"/>
       <c r="B70" s="53"/>
       <c r="C70" s="56" t="s">
@@ -8047,7 +8053,7 @@
       <c r="BY70" s="38"/>
       <c r="BZ70" s="38"/>
     </row>
-    <row r="71" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A71" s="32"/>
       <c r="B71" s="53"/>
       <c r="C71" s="56" t="s">
@@ -8129,7 +8135,7 @@
       <c r="BY71" s="38"/>
       <c r="BZ71" s="38"/>
     </row>
-    <row r="72" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A72" s="32"/>
       <c r="B72" s="53"/>
       <c r="C72" s="56" t="s">
@@ -8211,7 +8217,7 @@
       <c r="BY72" s="38"/>
       <c r="BZ72" s="38"/>
     </row>
-    <row r="73" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A73" s="32"/>
       <c r="B73" s="53"/>
       <c r="C73" s="56" t="s">
@@ -8293,7 +8299,7 @@
       <c r="BY73" s="38"/>
       <c r="BZ73" s="38"/>
     </row>
-    <row r="74" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A74" s="32"/>
       <c r="B74" s="53"/>
       <c r="C74" s="56" t="s">
@@ -8375,7 +8381,7 @@
       <c r="BY74" s="38"/>
       <c r="BZ74" s="38"/>
     </row>
-    <row r="75" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A75" s="32"/>
       <c r="B75" s="53"/>
       <c r="C75" s="56" t="s">
@@ -8457,7 +8463,7 @@
       <c r="BY75" s="38"/>
       <c r="BZ75" s="38"/>
     </row>
-    <row r="76" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A76" s="32"/>
       <c r="B76" s="53"/>
       <c r="C76" s="56" t="s">
@@ -8501,9 +8507,9 @@
       <c r="AM76" s="38"/>
       <c r="AN76" s="38"/>
       <c r="AO76" s="38"/>
-      <c r="AP76" s="173"/>
-      <c r="AQ76" s="173"/>
-      <c r="AR76" s="173"/>
+      <c r="AP76" s="151"/>
+      <c r="AQ76" s="151"/>
+      <c r="AR76" s="151"/>
       <c r="AS76" s="40"/>
       <c r="AT76" s="40"/>
       <c r="AU76" s="150"/>
@@ -8539,7 +8545,7 @@
       <c r="BY76" s="38"/>
       <c r="BZ76" s="38"/>
     </row>
-    <row r="77" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A77" s="32"/>
       <c r="B77" s="53"/>
       <c r="C77" s="56"/>
@@ -8619,7 +8625,7 @@
       <c r="BY77" s="38"/>
       <c r="BZ77" s="38"/>
     </row>
-    <row r="78" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A78" s="72"/>
       <c r="B78" s="59"/>
       <c r="C78" s="60" t="s">
@@ -8701,7 +8707,7 @@
       <c r="BY78" s="67"/>
       <c r="BZ78" s="67"/>
     </row>
-    <row r="79" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A79" s="91"/>
       <c r="B79" s="92"/>
       <c r="C79" s="93" t="s">
@@ -8783,7 +8789,7 @@
       <c r="BY79" s="100"/>
       <c r="BZ79" s="100"/>
     </row>
-    <row r="80" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A80" s="32"/>
       <c r="B80" s="53"/>
       <c r="C80" s="56" t="s">
@@ -8865,7 +8871,7 @@
       <c r="BY80" s="38"/>
       <c r="BZ80" s="38"/>
     </row>
-    <row r="81" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A81" s="32"/>
       <c r="B81" s="53"/>
       <c r="C81" s="56" t="s">
@@ -8947,7 +8953,7 @@
       <c r="BY81" s="38"/>
       <c r="BZ81" s="38"/>
     </row>
-    <row r="82" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A82" s="32"/>
       <c r="B82" s="53"/>
       <c r="C82" s="56" t="s">
@@ -8995,9 +9001,9 @@
       <c r="AQ82" s="38"/>
       <c r="AR82" s="40"/>
       <c r="AS82" s="40"/>
-      <c r="AT82" s="40"/>
-      <c r="AU82" s="40"/>
-      <c r="AV82" s="40"/>
+      <c r="AT82" s="150"/>
+      <c r="AU82" s="150"/>
+      <c r="AV82" s="147"/>
       <c r="AW82" s="38"/>
       <c r="AX82" s="38"/>
       <c r="AY82" s="38"/>
@@ -9029,7 +9035,7 @@
       <c r="BY82" s="38"/>
       <c r="BZ82" s="38"/>
     </row>
-    <row r="83" spans="1:78" ht="16.8" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:78" ht="16.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A83" s="32"/>
       <c r="B83" s="53"/>
       <c r="C83" s="56" t="s">
@@ -9111,7 +9117,7 @@
       <c r="BY83" s="38"/>
       <c r="BZ83" s="38"/>
     </row>
-    <row r="84" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A84" s="32"/>
       <c r="B84" s="53"/>
       <c r="C84" s="56" t="s">
@@ -9193,7 +9199,7 @@
       <c r="BY84" s="38"/>
       <c r="BZ84" s="38"/>
     </row>
-    <row r="85" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A85" s="32"/>
       <c r="B85" s="53"/>
       <c r="C85" s="56" t="s">
@@ -9275,7 +9281,7 @@
       <c r="BY85" s="38"/>
       <c r="BZ85" s="38"/>
     </row>
-    <row r="86" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A86" s="32"/>
       <c r="B86" s="53"/>
       <c r="C86" s="56" t="s">
@@ -9357,7 +9363,7 @@
       <c r="BY86" s="38"/>
       <c r="BZ86" s="38"/>
     </row>
-    <row r="87" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A87" s="32"/>
       <c r="B87" s="53"/>
       <c r="C87" s="56" t="s">
@@ -9439,7 +9445,7 @@
       <c r="BY87" s="38"/>
       <c r="BZ87" s="38"/>
     </row>
-    <row r="88" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A88" s="32"/>
       <c r="B88" s="53"/>
       <c r="C88" s="57" t="s">
@@ -9480,7 +9486,7 @@
       <c r="AJ88" s="38"/>
       <c r="AK88" s="38"/>
       <c r="AL88" s="38"/>
-      <c r="AM88" s="173"/>
+      <c r="AM88" s="151"/>
       <c r="AN88" s="38"/>
       <c r="AO88" s="38"/>
       <c r="AP88" s="38"/>
@@ -9521,7 +9527,7 @@
       <c r="BY88" s="38"/>
       <c r="BZ88" s="38"/>
     </row>
-    <row r="89" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A89" s="32"/>
       <c r="B89" s="53"/>
       <c r="C89" s="56" t="s">
@@ -9603,93 +9609,93 @@
       <c r="BY89" s="38"/>
       <c r="BZ89" s="38"/>
     </row>
-    <row r="90" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="91"/>
-      <c r="B90" s="92"/>
-      <c r="C90" s="93" t="s">
-        <v>85</v>
-      </c>
-      <c r="D90" s="94"/>
-      <c r="E90" s="95"/>
-      <c r="F90" s="95"/>
-      <c r="G90" s="96"/>
-      <c r="H90" s="97"/>
-      <c r="I90" s="98"/>
-      <c r="J90" s="99"/>
-      <c r="K90" s="100"/>
-      <c r="L90" s="100"/>
-      <c r="M90" s="100"/>
-      <c r="N90" s="101"/>
-      <c r="O90" s="101"/>
-      <c r="P90" s="101"/>
-      <c r="Q90" s="101"/>
-      <c r="R90" s="101"/>
-      <c r="S90" s="100"/>
-      <c r="T90" s="100"/>
-      <c r="U90" s="100"/>
-      <c r="V90" s="100"/>
-      <c r="W90" s="100"/>
-      <c r="X90" s="100"/>
-      <c r="Y90" s="100"/>
-      <c r="Z90" s="100"/>
-      <c r="AA90" s="100"/>
-      <c r="AB90" s="100"/>
-      <c r="AC90" s="102"/>
-      <c r="AD90" s="102"/>
-      <c r="AE90" s="102"/>
-      <c r="AF90" s="102"/>
-      <c r="AG90" s="102"/>
-      <c r="AH90" s="100"/>
-      <c r="AI90" s="100"/>
-      <c r="AJ90" s="100"/>
-      <c r="AK90" s="100"/>
-      <c r="AL90" s="100"/>
-      <c r="AM90" s="100"/>
-      <c r="AN90" s="100"/>
-      <c r="AO90" s="100"/>
-      <c r="AP90" s="100"/>
-      <c r="AQ90" s="100"/>
-      <c r="AR90" s="103"/>
-      <c r="AS90" s="103"/>
-      <c r="AT90" s="103"/>
-      <c r="AU90" s="103"/>
-      <c r="AV90" s="103"/>
-      <c r="AW90" s="100"/>
-      <c r="AX90" s="100"/>
-      <c r="AY90" s="100"/>
-      <c r="AZ90" s="100"/>
-      <c r="BA90" s="100"/>
-      <c r="BB90" s="100"/>
-      <c r="BC90" s="100"/>
-      <c r="BD90" s="100"/>
-      <c r="BE90" s="100"/>
-      <c r="BF90" s="100"/>
-      <c r="BG90" s="104"/>
-      <c r="BH90" s="104"/>
-      <c r="BI90" s="104"/>
-      <c r="BJ90" s="104"/>
-      <c r="BK90" s="104"/>
-      <c r="BL90" s="100"/>
-      <c r="BM90" s="100"/>
-      <c r="BN90" s="100"/>
-      <c r="BO90" s="100"/>
-      <c r="BP90" s="100"/>
-      <c r="BQ90" s="100"/>
-      <c r="BR90" s="100"/>
-      <c r="BS90" s="100"/>
-      <c r="BT90" s="100"/>
-      <c r="BU90" s="100"/>
-      <c r="BV90" s="100"/>
-      <c r="BW90" s="100"/>
-      <c r="BX90" s="100"/>
-      <c r="BY90" s="100"/>
-      <c r="BZ90" s="100"/>
+    <row r="90" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="32"/>
+      <c r="B90" s="53"/>
+      <c r="C90" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D90" s="54"/>
+      <c r="E90" s="35"/>
+      <c r="F90" s="35"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="37"/>
+      <c r="I90" s="42"/>
+      <c r="J90" s="43"/>
+      <c r="K90" s="38"/>
+      <c r="L90" s="38"/>
+      <c r="M90" s="38"/>
+      <c r="N90" s="44"/>
+      <c r="O90" s="44"/>
+      <c r="P90" s="44"/>
+      <c r="Q90" s="44"/>
+      <c r="R90" s="44"/>
+      <c r="S90" s="38"/>
+      <c r="T90" s="38"/>
+      <c r="U90" s="38"/>
+      <c r="V90" s="38"/>
+      <c r="W90" s="38"/>
+      <c r="X90" s="38"/>
+      <c r="Y90" s="38"/>
+      <c r="Z90" s="38"/>
+      <c r="AA90" s="38"/>
+      <c r="AB90" s="38"/>
+      <c r="AC90" s="39"/>
+      <c r="AD90" s="39"/>
+      <c r="AE90" s="39"/>
+      <c r="AF90" s="39"/>
+      <c r="AG90" s="39"/>
+      <c r="AH90" s="38"/>
+      <c r="AI90" s="38"/>
+      <c r="AJ90" s="38"/>
+      <c r="AK90" s="38"/>
+      <c r="AL90" s="38"/>
+      <c r="AM90" s="38"/>
+      <c r="AN90" s="38"/>
+      <c r="AO90" s="38"/>
+      <c r="AP90" s="38"/>
+      <c r="AQ90" s="38"/>
+      <c r="AR90" s="150"/>
+      <c r="AS90" s="150"/>
+      <c r="AT90" s="150"/>
+      <c r="AU90" s="150"/>
+      <c r="AV90" s="147"/>
+      <c r="AW90" s="38"/>
+      <c r="AX90" s="38"/>
+      <c r="AY90" s="38"/>
+      <c r="AZ90" s="38"/>
+      <c r="BA90" s="38"/>
+      <c r="BB90" s="38"/>
+      <c r="BC90" s="38"/>
+      <c r="BD90" s="38"/>
+      <c r="BE90" s="38"/>
+      <c r="BF90" s="38"/>
+      <c r="BG90" s="41"/>
+      <c r="BH90" s="41"/>
+      <c r="BI90" s="41"/>
+      <c r="BJ90" s="41"/>
+      <c r="BK90" s="41"/>
+      <c r="BL90" s="38"/>
+      <c r="BM90" s="38"/>
+      <c r="BN90" s="38"/>
+      <c r="BO90" s="38"/>
+      <c r="BP90" s="38"/>
+      <c r="BQ90" s="38"/>
+      <c r="BR90" s="38"/>
+      <c r="BS90" s="38"/>
+      <c r="BT90" s="38"/>
+      <c r="BU90" s="38"/>
+      <c r="BV90" s="38"/>
+      <c r="BW90" s="38"/>
+      <c r="BX90" s="38"/>
+      <c r="BY90" s="38"/>
+      <c r="BZ90" s="38"/>
     </row>
-    <row r="91" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A91" s="32"/>
       <c r="B91" s="53"/>
       <c r="C91" s="56" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="D91" s="54"/>
       <c r="E91" s="35"/>
@@ -9701,11 +9707,11 @@
       <c r="K91" s="38"/>
       <c r="L91" s="38"/>
       <c r="M91" s="38"/>
-      <c r="N91" s="38"/>
-      <c r="O91" s="38"/>
-      <c r="P91" s="38"/>
-      <c r="Q91" s="38"/>
-      <c r="R91" s="38"/>
+      <c r="N91" s="44"/>
+      <c r="O91" s="44"/>
+      <c r="P91" s="44"/>
+      <c r="Q91" s="44"/>
+      <c r="R91" s="44"/>
       <c r="S91" s="38"/>
       <c r="T91" s="38"/>
       <c r="U91" s="38"/>
@@ -9716,26 +9722,26 @@
       <c r="Z91" s="38"/>
       <c r="AA91" s="38"/>
       <c r="AB91" s="38"/>
-      <c r="AC91" s="38"/>
-      <c r="AD91" s="38"/>
-      <c r="AE91" s="38"/>
-      <c r="AF91" s="38"/>
-      <c r="AG91" s="38"/>
+      <c r="AC91" s="39"/>
+      <c r="AD91" s="39"/>
+      <c r="AE91" s="39"/>
+      <c r="AF91" s="39"/>
+      <c r="AG91" s="39"/>
       <c r="AH91" s="38"/>
-      <c r="AI91" s="124"/>
-      <c r="AJ91" s="124"/>
-      <c r="AK91" s="124"/>
-      <c r="AL91" s="124"/>
-      <c r="AM91" s="58"/>
+      <c r="AI91" s="38"/>
+      <c r="AJ91" s="38"/>
+      <c r="AK91" s="38"/>
+      <c r="AL91" s="38"/>
+      <c r="AM91" s="38"/>
       <c r="AN91" s="38"/>
       <c r="AO91" s="38"/>
       <c r="AP91" s="38"/>
       <c r="AQ91" s="38"/>
-      <c r="AR91" s="38"/>
-      <c r="AS91" s="38"/>
-      <c r="AT91" s="38"/>
-      <c r="AU91" s="38"/>
-      <c r="AV91" s="38"/>
+      <c r="AR91" s="150"/>
+      <c r="AS91" s="150"/>
+      <c r="AT91" s="150"/>
+      <c r="AU91" s="150"/>
+      <c r="AV91" s="147"/>
       <c r="AW91" s="38"/>
       <c r="AX91" s="38"/>
       <c r="AY91" s="38"/>
@@ -9746,11 +9752,11 @@
       <c r="BD91" s="38"/>
       <c r="BE91" s="38"/>
       <c r="BF91" s="38"/>
-      <c r="BG91" s="38"/>
-      <c r="BH91" s="38"/>
-      <c r="BI91" s="38"/>
-      <c r="BJ91" s="38"/>
-      <c r="BK91" s="38"/>
+      <c r="BG91" s="41"/>
+      <c r="BH91" s="41"/>
+      <c r="BI91" s="41"/>
+      <c r="BJ91" s="41"/>
+      <c r="BK91" s="41"/>
       <c r="BL91" s="38"/>
       <c r="BM91" s="38"/>
       <c r="BN91" s="38"/>
@@ -9767,11 +9773,11 @@
       <c r="BY91" s="38"/>
       <c r="BZ91" s="38"/>
     </row>
-    <row r="92" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A92" s="32"/>
       <c r="B92" s="53"/>
       <c r="C92" s="56" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="D92" s="54"/>
       <c r="E92" s="35"/>
@@ -9783,11 +9789,11 @@
       <c r="K92" s="38"/>
       <c r="L92" s="38"/>
       <c r="M92" s="38"/>
-      <c r="N92" s="38"/>
-      <c r="O92" s="38"/>
-      <c r="P92" s="38"/>
-      <c r="Q92" s="38"/>
-      <c r="R92" s="38"/>
+      <c r="N92" s="44"/>
+      <c r="O92" s="44"/>
+      <c r="P92" s="44"/>
+      <c r="Q92" s="44"/>
+      <c r="R92" s="44"/>
       <c r="S92" s="38"/>
       <c r="T92" s="38"/>
       <c r="U92" s="38"/>
@@ -9798,11 +9804,11 @@
       <c r="Z92" s="38"/>
       <c r="AA92" s="38"/>
       <c r="AB92" s="38"/>
-      <c r="AC92" s="38"/>
-      <c r="AD92" s="38"/>
-      <c r="AE92" s="38"/>
-      <c r="AF92" s="38"/>
-      <c r="AG92" s="38"/>
+      <c r="AC92" s="39"/>
+      <c r="AD92" s="39"/>
+      <c r="AE92" s="39"/>
+      <c r="AF92" s="39"/>
+      <c r="AG92" s="39"/>
       <c r="AH92" s="38"/>
       <c r="AI92" s="38"/>
       <c r="AJ92" s="38"/>
@@ -9813,11 +9819,11 @@
       <c r="AO92" s="38"/>
       <c r="AP92" s="38"/>
       <c r="AQ92" s="38"/>
-      <c r="AR92" s="38"/>
-      <c r="AS92" s="38"/>
-      <c r="AT92" s="38"/>
-      <c r="AU92" s="38"/>
-      <c r="AV92" s="38"/>
+      <c r="AR92" s="150"/>
+      <c r="AS92" s="150"/>
+      <c r="AT92" s="150"/>
+      <c r="AU92" s="150"/>
+      <c r="AV92" s="147"/>
       <c r="AW92" s="38"/>
       <c r="AX92" s="38"/>
       <c r="AY92" s="38"/>
@@ -9828,11 +9834,11 @@
       <c r="BD92" s="38"/>
       <c r="BE92" s="38"/>
       <c r="BF92" s="38"/>
-      <c r="BG92" s="38"/>
-      <c r="BH92" s="38"/>
-      <c r="BI92" s="38"/>
-      <c r="BJ92" s="38"/>
-      <c r="BK92" s="38"/>
+      <c r="BG92" s="41"/>
+      <c r="BH92" s="41"/>
+      <c r="BI92" s="41"/>
+      <c r="BJ92" s="41"/>
+      <c r="BK92" s="41"/>
       <c r="BL92" s="38"/>
       <c r="BM92" s="38"/>
       <c r="BN92" s="38"/>
@@ -9849,92 +9855,94 @@
       <c r="BY92" s="38"/>
       <c r="BZ92" s="38"/>
     </row>
-    <row r="93" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="32"/>
-      <c r="B93" s="53"/>
-      <c r="C93" s="56" t="s">
-        <v>131</v>
-      </c>
-      <c r="D93" s="54"/>
-      <c r="E93" s="35"/>
-      <c r="F93" s="35"/>
-      <c r="G93" s="36"/>
-      <c r="H93" s="37"/>
-      <c r="I93" s="42"/>
-      <c r="J93" s="43"/>
-      <c r="K93" s="38"/>
-      <c r="L93" s="38"/>
-      <c r="M93" s="38"/>
-      <c r="N93" s="38"/>
-      <c r="O93" s="38"/>
-      <c r="P93" s="38"/>
-      <c r="Q93" s="38"/>
-      <c r="R93" s="38"/>
-      <c r="S93" s="38"/>
-      <c r="T93" s="38"/>
-      <c r="U93" s="38"/>
-      <c r="V93" s="38"/>
-      <c r="W93" s="38"/>
-      <c r="X93" s="38"/>
-      <c r="Y93" s="38"/>
-      <c r="Z93" s="38"/>
-      <c r="AA93" s="38"/>
-      <c r="AB93" s="38"/>
-      <c r="AC93" s="38"/>
-      <c r="AD93" s="38"/>
-      <c r="AE93" s="38"/>
-      <c r="AF93" s="38"/>
-      <c r="AG93" s="38"/>
-      <c r="AH93" s="38"/>
-      <c r="AI93" s="38"/>
-      <c r="AJ93" s="38"/>
-      <c r="AK93" s="38"/>
-      <c r="AL93" s="38"/>
-      <c r="AM93" s="38"/>
-      <c r="AN93" s="38"/>
-      <c r="AO93" s="38"/>
-      <c r="AP93" s="38"/>
-      <c r="AQ93" s="38"/>
-      <c r="AR93" s="124"/>
-      <c r="AS93" s="124"/>
-      <c r="AT93" s="124"/>
-      <c r="AU93" s="124"/>
-      <c r="AV93" s="124"/>
-      <c r="AW93" s="58"/>
-      <c r="AX93" s="38"/>
-      <c r="AY93" s="38"/>
-      <c r="AZ93" s="38"/>
-      <c r="BA93" s="38"/>
-      <c r="BB93" s="38"/>
-      <c r="BC93" s="38"/>
-      <c r="BD93" s="38"/>
-      <c r="BE93" s="38"/>
-      <c r="BF93" s="38"/>
-      <c r="BG93" s="38"/>
-      <c r="BH93" s="38"/>
-      <c r="BI93" s="38"/>
-      <c r="BJ93" s="38"/>
-      <c r="BK93" s="38"/>
-      <c r="BL93" s="38"/>
-      <c r="BM93" s="38"/>
-      <c r="BN93" s="38"/>
-      <c r="BO93" s="38"/>
-      <c r="BP93" s="38"/>
-      <c r="BQ93" s="38"/>
-      <c r="BR93" s="38"/>
-      <c r="BS93" s="38"/>
-      <c r="BT93" s="38"/>
-      <c r="BU93" s="38"/>
-      <c r="BV93" s="38"/>
-      <c r="BW93" s="38"/>
-      <c r="BX93" s="38"/>
-      <c r="BY93" s="38"/>
-      <c r="BZ93" s="38"/>
+    <row r="93" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="91"/>
+      <c r="B93" s="92"/>
+      <c r="C93" s="93" t="s">
+        <v>85</v>
+      </c>
+      <c r="D93" s="94"/>
+      <c r="E93" s="95"/>
+      <c r="F93" s="95"/>
+      <c r="G93" s="96"/>
+      <c r="H93" s="97"/>
+      <c r="I93" s="98"/>
+      <c r="J93" s="99"/>
+      <c r="K93" s="100"/>
+      <c r="L93" s="100"/>
+      <c r="M93" s="100"/>
+      <c r="N93" s="101"/>
+      <c r="O93" s="101"/>
+      <c r="P93" s="101"/>
+      <c r="Q93" s="101"/>
+      <c r="R93" s="101"/>
+      <c r="S93" s="100"/>
+      <c r="T93" s="100"/>
+      <c r="U93" s="100"/>
+      <c r="V93" s="100"/>
+      <c r="W93" s="100"/>
+      <c r="X93" s="100"/>
+      <c r="Y93" s="100"/>
+      <c r="Z93" s="100"/>
+      <c r="AA93" s="100"/>
+      <c r="AB93" s="100"/>
+      <c r="AC93" s="102"/>
+      <c r="AD93" s="102"/>
+      <c r="AE93" s="102"/>
+      <c r="AF93" s="102"/>
+      <c r="AG93" s="102"/>
+      <c r="AH93" s="100"/>
+      <c r="AI93" s="100"/>
+      <c r="AJ93" s="100"/>
+      <c r="AK93" s="100"/>
+      <c r="AL93" s="100"/>
+      <c r="AM93" s="100"/>
+      <c r="AN93" s="100"/>
+      <c r="AO93" s="100"/>
+      <c r="AP93" s="100"/>
+      <c r="AQ93" s="100"/>
+      <c r="AR93" s="103"/>
+      <c r="AS93" s="103"/>
+      <c r="AT93" s="103"/>
+      <c r="AU93" s="103"/>
+      <c r="AV93" s="103"/>
+      <c r="AW93" s="100"/>
+      <c r="AX93" s="100"/>
+      <c r="AY93" s="100"/>
+      <c r="AZ93" s="100"/>
+      <c r="BA93" s="100"/>
+      <c r="BB93" s="100"/>
+      <c r="BC93" s="100"/>
+      <c r="BD93" s="100"/>
+      <c r="BE93" s="100"/>
+      <c r="BF93" s="100"/>
+      <c r="BG93" s="104"/>
+      <c r="BH93" s="104"/>
+      <c r="BI93" s="104"/>
+      <c r="BJ93" s="104"/>
+      <c r="BK93" s="104"/>
+      <c r="BL93" s="100"/>
+      <c r="BM93" s="100"/>
+      <c r="BN93" s="100"/>
+      <c r="BO93" s="100"/>
+      <c r="BP93" s="100"/>
+      <c r="BQ93" s="100"/>
+      <c r="BR93" s="100"/>
+      <c r="BS93" s="100"/>
+      <c r="BT93" s="100"/>
+      <c r="BU93" s="100"/>
+      <c r="BV93" s="100"/>
+      <c r="BW93" s="100"/>
+      <c r="BX93" s="100"/>
+      <c r="BY93" s="100"/>
+      <c r="BZ93" s="100"/>
     </row>
-    <row r="94" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A94" s="32"/>
       <c r="B94" s="53"/>
-      <c r="C94" s="56"/>
+      <c r="C94" s="56" t="s">
+        <v>90</v>
+      </c>
       <c r="D94" s="54"/>
       <c r="E94" s="35"/>
       <c r="F94" s="35"/>
@@ -9966,11 +9974,11 @@
       <c r="AF94" s="38"/>
       <c r="AG94" s="38"/>
       <c r="AH94" s="38"/>
-      <c r="AI94" s="38"/>
-      <c r="AJ94" s="38"/>
-      <c r="AK94" s="38"/>
-      <c r="AL94" s="38"/>
-      <c r="AM94" s="38"/>
+      <c r="AI94" s="124"/>
+      <c r="AJ94" s="124"/>
+      <c r="AK94" s="124"/>
+      <c r="AL94" s="124"/>
+      <c r="AM94" s="58"/>
       <c r="AN94" s="38"/>
       <c r="AO94" s="38"/>
       <c r="AP94" s="38"/>
@@ -10011,93 +10019,93 @@
       <c r="BY94" s="38"/>
       <c r="BZ94" s="38"/>
     </row>
-    <row r="95" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="72"/>
-      <c r="B95" s="59"/>
-      <c r="C95" s="77" t="s">
-        <v>38</v>
-      </c>
-      <c r="D95" s="61"/>
-      <c r="E95" s="62"/>
-      <c r="F95" s="62"/>
-      <c r="G95" s="63"/>
-      <c r="H95" s="64"/>
-      <c r="I95" s="65"/>
-      <c r="J95" s="66"/>
-      <c r="K95" s="67"/>
-      <c r="L95" s="67"/>
-      <c r="M95" s="67"/>
-      <c r="N95" s="68"/>
-      <c r="O95" s="68"/>
-      <c r="P95" s="68"/>
-      <c r="Q95" s="68"/>
-      <c r="R95" s="68"/>
-      <c r="S95" s="67"/>
-      <c r="T95" s="67"/>
-      <c r="U95" s="67"/>
-      <c r="V95" s="67"/>
-      <c r="W95" s="67"/>
-      <c r="X95" s="67"/>
-      <c r="Y95" s="67"/>
-      <c r="Z95" s="67"/>
-      <c r="AA95" s="67"/>
-      <c r="AB95" s="67"/>
-      <c r="AC95" s="69"/>
-      <c r="AD95" s="69"/>
-      <c r="AE95" s="69"/>
-      <c r="AF95" s="69"/>
-      <c r="AG95" s="69"/>
-      <c r="AH95" s="67"/>
-      <c r="AI95" s="67"/>
-      <c r="AJ95" s="67"/>
-      <c r="AK95" s="67"/>
-      <c r="AL95" s="67"/>
-      <c r="AM95" s="67"/>
-      <c r="AN95" s="67"/>
-      <c r="AO95" s="67"/>
-      <c r="AP95" s="67"/>
-      <c r="AQ95" s="67"/>
-      <c r="AR95" s="70"/>
-      <c r="AS95" s="70"/>
-      <c r="AT95" s="70"/>
-      <c r="AU95" s="70"/>
-      <c r="AV95" s="70"/>
-      <c r="AW95" s="67"/>
-      <c r="AX95" s="67"/>
-      <c r="AY95" s="67"/>
-      <c r="AZ95" s="67"/>
-      <c r="BA95" s="67"/>
-      <c r="BB95" s="67"/>
-      <c r="BC95" s="67"/>
-      <c r="BD95" s="67"/>
-      <c r="BE95" s="67"/>
-      <c r="BF95" s="67"/>
-      <c r="BG95" s="71"/>
-      <c r="BH95" s="71"/>
-      <c r="BI95" s="71"/>
-      <c r="BJ95" s="71"/>
-      <c r="BK95" s="71"/>
-      <c r="BL95" s="67"/>
-      <c r="BM95" s="67"/>
-      <c r="BN95" s="67"/>
-      <c r="BO95" s="67"/>
-      <c r="BP95" s="67"/>
-      <c r="BQ95" s="67"/>
-      <c r="BR95" s="67"/>
-      <c r="BS95" s="67"/>
-      <c r="BT95" s="67"/>
-      <c r="BU95" s="67"/>
-      <c r="BV95" s="67"/>
-      <c r="BW95" s="67"/>
-      <c r="BX95" s="67"/>
-      <c r="BY95" s="67"/>
-      <c r="BZ95" s="67"/>
+    <row r="95" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="32"/>
+      <c r="B95" s="53"/>
+      <c r="C95" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D95" s="54"/>
+      <c r="E95" s="35"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
+      <c r="I95" s="42"/>
+      <c r="J95" s="43"/>
+      <c r="K95" s="38"/>
+      <c r="L95" s="38"/>
+      <c r="M95" s="38"/>
+      <c r="N95" s="38"/>
+      <c r="O95" s="38"/>
+      <c r="P95" s="38"/>
+      <c r="Q95" s="38"/>
+      <c r="R95" s="38"/>
+      <c r="S95" s="38"/>
+      <c r="T95" s="38"/>
+      <c r="U95" s="38"/>
+      <c r="V95" s="38"/>
+      <c r="W95" s="38"/>
+      <c r="X95" s="38"/>
+      <c r="Y95" s="38"/>
+      <c r="Z95" s="38"/>
+      <c r="AA95" s="38"/>
+      <c r="AB95" s="38"/>
+      <c r="AC95" s="38"/>
+      <c r="AD95" s="38"/>
+      <c r="AE95" s="38"/>
+      <c r="AF95" s="38"/>
+      <c r="AG95" s="38"/>
+      <c r="AH95" s="38"/>
+      <c r="AI95" s="38"/>
+      <c r="AJ95" s="38"/>
+      <c r="AK95" s="38"/>
+      <c r="AL95" s="38"/>
+      <c r="AM95" s="38"/>
+      <c r="AN95" s="38"/>
+      <c r="AO95" s="38"/>
+      <c r="AP95" s="38"/>
+      <c r="AQ95" s="38"/>
+      <c r="AR95" s="38"/>
+      <c r="AS95" s="38"/>
+      <c r="AT95" s="38"/>
+      <c r="AU95" s="38"/>
+      <c r="AV95" s="38"/>
+      <c r="AW95" s="38"/>
+      <c r="AX95" s="38"/>
+      <c r="AY95" s="38"/>
+      <c r="AZ95" s="38"/>
+      <c r="BA95" s="38"/>
+      <c r="BB95" s="38"/>
+      <c r="BC95" s="38"/>
+      <c r="BD95" s="38"/>
+      <c r="BE95" s="38"/>
+      <c r="BF95" s="38"/>
+      <c r="BG95" s="38"/>
+      <c r="BH95" s="38"/>
+      <c r="BI95" s="38"/>
+      <c r="BJ95" s="38"/>
+      <c r="BK95" s="38"/>
+      <c r="BL95" s="38"/>
+      <c r="BM95" s="38"/>
+      <c r="BN95" s="38"/>
+      <c r="BO95" s="38"/>
+      <c r="BP95" s="38"/>
+      <c r="BQ95" s="38"/>
+      <c r="BR95" s="38"/>
+      <c r="BS95" s="38"/>
+      <c r="BT95" s="38"/>
+      <c r="BU95" s="38"/>
+      <c r="BV95" s="38"/>
+      <c r="BW95" s="38"/>
+      <c r="BX95" s="38"/>
+      <c r="BY95" s="38"/>
+      <c r="BZ95" s="38"/>
     </row>
-    <row r="96" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A96" s="32"/>
       <c r="B96" s="53"/>
       <c r="C96" s="56" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="D96" s="54"/>
       <c r="E96" s="35"/>
@@ -10109,11 +10117,11 @@
       <c r="K96" s="38"/>
       <c r="L96" s="38"/>
       <c r="M96" s="38"/>
-      <c r="N96" s="44"/>
-      <c r="O96" s="44"/>
-      <c r="P96" s="44"/>
-      <c r="Q96" s="44"/>
-      <c r="R96" s="44"/>
+      <c r="N96" s="38"/>
+      <c r="O96" s="38"/>
+      <c r="P96" s="38"/>
+      <c r="Q96" s="38"/>
+      <c r="R96" s="38"/>
       <c r="S96" s="38"/>
       <c r="T96" s="38"/>
       <c r="U96" s="38"/>
@@ -10124,27 +10132,27 @@
       <c r="Z96" s="38"/>
       <c r="AA96" s="38"/>
       <c r="AB96" s="38"/>
-      <c r="AC96" s="39"/>
-      <c r="AD96" s="39"/>
-      <c r="AE96" s="39"/>
-      <c r="AF96" s="39"/>
-      <c r="AG96" s="39"/>
-      <c r="AH96" s="124"/>
-      <c r="AI96" s="124"/>
-      <c r="AJ96" s="124"/>
-      <c r="AK96" s="124"/>
-      <c r="AL96" s="124"/>
-      <c r="AM96" s="58"/>
+      <c r="AC96" s="38"/>
+      <c r="AD96" s="38"/>
+      <c r="AE96" s="38"/>
+      <c r="AF96" s="38"/>
+      <c r="AG96" s="38"/>
+      <c r="AH96" s="38"/>
+      <c r="AI96" s="38"/>
+      <c r="AJ96" s="38"/>
+      <c r="AK96" s="38"/>
+      <c r="AL96" s="38"/>
+      <c r="AM96" s="38"/>
       <c r="AN96" s="38"/>
       <c r="AO96" s="38"/>
       <c r="AP96" s="38"/>
       <c r="AQ96" s="38"/>
-      <c r="AR96" s="40"/>
-      <c r="AS96" s="40"/>
-      <c r="AT96" s="40"/>
-      <c r="AU96" s="40"/>
-      <c r="AV96" s="40"/>
-      <c r="AW96" s="38"/>
+      <c r="AR96" s="124"/>
+      <c r="AS96" s="124"/>
+      <c r="AT96" s="124"/>
+      <c r="AU96" s="124"/>
+      <c r="AV96" s="124"/>
+      <c r="AW96" s="58"/>
       <c r="AX96" s="38"/>
       <c r="AY96" s="38"/>
       <c r="AZ96" s="38"/>
@@ -10154,11 +10162,11 @@
       <c r="BD96" s="38"/>
       <c r="BE96" s="38"/>
       <c r="BF96" s="38"/>
-      <c r="BG96" s="41"/>
-      <c r="BH96" s="41"/>
-      <c r="BI96" s="41"/>
-      <c r="BJ96" s="41"/>
-      <c r="BK96" s="41"/>
+      <c r="BG96" s="38"/>
+      <c r="BH96" s="38"/>
+      <c r="BI96" s="38"/>
+      <c r="BJ96" s="38"/>
+      <c r="BK96" s="38"/>
       <c r="BL96" s="38"/>
       <c r="BM96" s="38"/>
       <c r="BN96" s="38"/>
@@ -10175,12 +10183,10 @@
       <c r="BY96" s="38"/>
       <c r="BZ96" s="38"/>
     </row>
-    <row r="97" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A97" s="32"/>
       <c r="B97" s="53"/>
-      <c r="C97" s="56" t="s">
-        <v>80</v>
-      </c>
+      <c r="C97" s="56"/>
       <c r="D97" s="54"/>
       <c r="E97" s="35"/>
       <c r="F97" s="35"/>
@@ -10191,11 +10197,11 @@
       <c r="K97" s="38"/>
       <c r="L97" s="38"/>
       <c r="M97" s="38"/>
-      <c r="N97" s="44"/>
-      <c r="O97" s="44"/>
-      <c r="P97" s="44"/>
-      <c r="Q97" s="44"/>
-      <c r="R97" s="44"/>
+      <c r="N97" s="38"/>
+      <c r="O97" s="38"/>
+      <c r="P97" s="38"/>
+      <c r="Q97" s="38"/>
+      <c r="R97" s="38"/>
       <c r="S97" s="38"/>
       <c r="T97" s="38"/>
       <c r="U97" s="38"/>
@@ -10206,26 +10212,26 @@
       <c r="Z97" s="38"/>
       <c r="AA97" s="38"/>
       <c r="AB97" s="38"/>
-      <c r="AC97" s="39"/>
-      <c r="AD97" s="39"/>
-      <c r="AE97" s="39"/>
-      <c r="AF97" s="39"/>
-      <c r="AG97" s="39"/>
-      <c r="AH97" s="124"/>
-      <c r="AI97" s="124"/>
-      <c r="AJ97" s="124"/>
-      <c r="AK97" s="124"/>
-      <c r="AL97" s="124"/>
-      <c r="AM97" s="58"/>
+      <c r="AC97" s="38"/>
+      <c r="AD97" s="38"/>
+      <c r="AE97" s="38"/>
+      <c r="AF97" s="38"/>
+      <c r="AG97" s="38"/>
+      <c r="AH97" s="38"/>
+      <c r="AI97" s="38"/>
+      <c r="AJ97" s="38"/>
+      <c r="AK97" s="38"/>
+      <c r="AL97" s="38"/>
+      <c r="AM97" s="38"/>
       <c r="AN97" s="38"/>
       <c r="AO97" s="38"/>
       <c r="AP97" s="38"/>
       <c r="AQ97" s="38"/>
-      <c r="AR97" s="40"/>
-      <c r="AS97" s="40"/>
-      <c r="AT97" s="40"/>
-      <c r="AU97" s="40"/>
-      <c r="AV97" s="40"/>
+      <c r="AR97" s="38"/>
+      <c r="AS97" s="38"/>
+      <c r="AT97" s="38"/>
+      <c r="AU97" s="38"/>
+      <c r="AV97" s="38"/>
       <c r="AW97" s="38"/>
       <c r="AX97" s="38"/>
       <c r="AY97" s="38"/>
@@ -10236,11 +10242,11 @@
       <c r="BD97" s="38"/>
       <c r="BE97" s="38"/>
       <c r="BF97" s="38"/>
-      <c r="BG97" s="41"/>
-      <c r="BH97" s="41"/>
-      <c r="BI97" s="41"/>
-      <c r="BJ97" s="41"/>
-      <c r="BK97" s="41"/>
+      <c r="BG97" s="38"/>
+      <c r="BH97" s="38"/>
+      <c r="BI97" s="38"/>
+      <c r="BJ97" s="38"/>
+      <c r="BK97" s="38"/>
       <c r="BL97" s="38"/>
       <c r="BM97" s="38"/>
       <c r="BN97" s="38"/>
@@ -10257,93 +10263,93 @@
       <c r="BY97" s="38"/>
       <c r="BZ97" s="38"/>
     </row>
-    <row r="98" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="32"/>
-      <c r="B98" s="53"/>
-      <c r="C98" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="D98" s="54"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="35"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="37"/>
-      <c r="I98" s="42"/>
-      <c r="J98" s="43"/>
-      <c r="K98" s="38"/>
-      <c r="L98" s="38"/>
-      <c r="M98" s="38"/>
-      <c r="N98" s="44"/>
-      <c r="O98" s="44"/>
-      <c r="P98" s="44"/>
-      <c r="Q98" s="44"/>
-      <c r="R98" s="44"/>
-      <c r="S98" s="38"/>
-      <c r="T98" s="38"/>
-      <c r="U98" s="38"/>
-      <c r="V98" s="38"/>
-      <c r="W98" s="38"/>
-      <c r="X98" s="38"/>
-      <c r="Y98" s="38"/>
-      <c r="Z98" s="38"/>
-      <c r="AA98" s="38"/>
-      <c r="AB98" s="38"/>
-      <c r="AC98" s="39"/>
-      <c r="AD98" s="39"/>
-      <c r="AE98" s="39"/>
-      <c r="AF98" s="39"/>
-      <c r="AG98" s="39"/>
-      <c r="AH98" s="38"/>
-      <c r="AI98" s="38"/>
-      <c r="AJ98" s="38"/>
-      <c r="AK98" s="38"/>
-      <c r="AL98" s="38"/>
-      <c r="AM98" s="38"/>
-      <c r="AN98" s="38"/>
-      <c r="AO98" s="149"/>
-      <c r="AP98" s="149"/>
-      <c r="AQ98" s="149"/>
-      <c r="AR98" s="147"/>
-      <c r="AS98" s="40"/>
-      <c r="AT98" s="40"/>
-      <c r="AU98" s="40"/>
-      <c r="AV98" s="40"/>
-      <c r="AW98" s="38"/>
-      <c r="AX98" s="38"/>
-      <c r="AY98" s="38"/>
-      <c r="AZ98" s="38"/>
-      <c r="BA98" s="38"/>
-      <c r="BB98" s="38"/>
-      <c r="BC98" s="38"/>
-      <c r="BD98" s="38"/>
-      <c r="BE98" s="38"/>
-      <c r="BF98" s="38"/>
-      <c r="BG98" s="41"/>
-      <c r="BH98" s="41"/>
-      <c r="BI98" s="41"/>
-      <c r="BJ98" s="41"/>
-      <c r="BK98" s="41"/>
-      <c r="BL98" s="38"/>
-      <c r="BM98" s="38"/>
-      <c r="BN98" s="38"/>
-      <c r="BO98" s="38"/>
-      <c r="BP98" s="38"/>
-      <c r="BQ98" s="38"/>
-      <c r="BR98" s="38"/>
-      <c r="BS98" s="38"/>
-      <c r="BT98" s="38"/>
-      <c r="BU98" s="38"/>
-      <c r="BV98" s="38"/>
-      <c r="BW98" s="38"/>
-      <c r="BX98" s="38"/>
-      <c r="BY98" s="38"/>
-      <c r="BZ98" s="38"/>
+    <row r="98" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="72"/>
+      <c r="B98" s="59"/>
+      <c r="C98" s="77" t="s">
+        <v>38</v>
+      </c>
+      <c r="D98" s="61"/>
+      <c r="E98" s="62"/>
+      <c r="F98" s="62"/>
+      <c r="G98" s="63"/>
+      <c r="H98" s="64"/>
+      <c r="I98" s="65"/>
+      <c r="J98" s="66"/>
+      <c r="K98" s="67"/>
+      <c r="L98" s="67"/>
+      <c r="M98" s="67"/>
+      <c r="N98" s="68"/>
+      <c r="O98" s="68"/>
+      <c r="P98" s="68"/>
+      <c r="Q98" s="68"/>
+      <c r="R98" s="68"/>
+      <c r="S98" s="67"/>
+      <c r="T98" s="67"/>
+      <c r="U98" s="67"/>
+      <c r="V98" s="67"/>
+      <c r="W98" s="67"/>
+      <c r="X98" s="67"/>
+      <c r="Y98" s="67"/>
+      <c r="Z98" s="67"/>
+      <c r="AA98" s="67"/>
+      <c r="AB98" s="67"/>
+      <c r="AC98" s="69"/>
+      <c r="AD98" s="69"/>
+      <c r="AE98" s="69"/>
+      <c r="AF98" s="69"/>
+      <c r="AG98" s="69"/>
+      <c r="AH98" s="67"/>
+      <c r="AI98" s="67"/>
+      <c r="AJ98" s="67"/>
+      <c r="AK98" s="67"/>
+      <c r="AL98" s="67"/>
+      <c r="AM98" s="67"/>
+      <c r="AN98" s="67"/>
+      <c r="AO98" s="67"/>
+      <c r="AP98" s="67"/>
+      <c r="AQ98" s="67"/>
+      <c r="AR98" s="70"/>
+      <c r="AS98" s="70"/>
+      <c r="AT98" s="70"/>
+      <c r="AU98" s="70"/>
+      <c r="AV98" s="70"/>
+      <c r="AW98" s="67"/>
+      <c r="AX98" s="67"/>
+      <c r="AY98" s="67"/>
+      <c r="AZ98" s="67"/>
+      <c r="BA98" s="67"/>
+      <c r="BB98" s="67"/>
+      <c r="BC98" s="67"/>
+      <c r="BD98" s="67"/>
+      <c r="BE98" s="67"/>
+      <c r="BF98" s="67"/>
+      <c r="BG98" s="71"/>
+      <c r="BH98" s="71"/>
+      <c r="BI98" s="71"/>
+      <c r="BJ98" s="71"/>
+      <c r="BK98" s="71"/>
+      <c r="BL98" s="67"/>
+      <c r="BM98" s="67"/>
+      <c r="BN98" s="67"/>
+      <c r="BO98" s="67"/>
+      <c r="BP98" s="67"/>
+      <c r="BQ98" s="67"/>
+      <c r="BR98" s="67"/>
+      <c r="BS98" s="67"/>
+      <c r="BT98" s="67"/>
+      <c r="BU98" s="67"/>
+      <c r="BV98" s="67"/>
+      <c r="BW98" s="67"/>
+      <c r="BX98" s="67"/>
+      <c r="BY98" s="67"/>
+      <c r="BZ98" s="67"/>
     </row>
-    <row r="99" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A99" s="32"/>
       <c r="B99" s="53"/>
       <c r="C99" s="56" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="D99" s="54"/>
       <c r="E99" s="35"/>
@@ -10375,22 +10381,22 @@
       <c r="AE99" s="39"/>
       <c r="AF99" s="39"/>
       <c r="AG99" s="39"/>
-      <c r="AH99" s="38"/>
-      <c r="AI99" s="38"/>
-      <c r="AJ99" s="38"/>
-      <c r="AK99" s="38"/>
-      <c r="AL99" s="38"/>
-      <c r="AM99" s="38"/>
+      <c r="AH99" s="124"/>
+      <c r="AI99" s="124"/>
+      <c r="AJ99" s="124"/>
+      <c r="AK99" s="124"/>
+      <c r="AL99" s="124"/>
+      <c r="AM99" s="58"/>
       <c r="AN99" s="38"/>
-      <c r="AO99" s="149"/>
-      <c r="AP99" s="149"/>
-      <c r="AQ99" s="149"/>
-      <c r="AR99" s="149"/>
-      <c r="AS99" s="149"/>
-      <c r="AT99" s="149"/>
-      <c r="AU99" s="149"/>
-      <c r="AV99" s="149"/>
-      <c r="AW99" s="58"/>
+      <c r="AO99" s="38"/>
+      <c r="AP99" s="38"/>
+      <c r="AQ99" s="38"/>
+      <c r="AR99" s="40"/>
+      <c r="AS99" s="40"/>
+      <c r="AT99" s="40"/>
+      <c r="AU99" s="40"/>
+      <c r="AV99" s="40"/>
+      <c r="AW99" s="38"/>
       <c r="AX99" s="38"/>
       <c r="AY99" s="38"/>
       <c r="AZ99" s="38"/>
@@ -10421,11 +10427,11 @@
       <c r="BY99" s="38"/>
       <c r="BZ99" s="38"/>
     </row>
-    <row r="100" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A100" s="32"/>
       <c r="B100" s="53"/>
       <c r="C100" s="56" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="D100" s="54"/>
       <c r="E100" s="35"/>
@@ -10457,17 +10463,17 @@
       <c r="AE100" s="39"/>
       <c r="AF100" s="39"/>
       <c r="AG100" s="39"/>
-      <c r="AH100" s="38"/>
-      <c r="AI100" s="38"/>
-      <c r="AJ100" s="38"/>
-      <c r="AK100" s="38"/>
-      <c r="AL100" s="38"/>
-      <c r="AM100" s="38"/>
+      <c r="AH100" s="124"/>
+      <c r="AI100" s="124"/>
+      <c r="AJ100" s="124"/>
+      <c r="AK100" s="124"/>
+      <c r="AL100" s="124"/>
+      <c r="AM100" s="58"/>
       <c r="AN100" s="38"/>
-      <c r="AO100" s="124"/>
-      <c r="AP100" s="124"/>
-      <c r="AQ100" s="150"/>
-      <c r="AR100" s="147"/>
+      <c r="AO100" s="38"/>
+      <c r="AP100" s="38"/>
+      <c r="AQ100" s="38"/>
+      <c r="AR100" s="40"/>
       <c r="AS100" s="40"/>
       <c r="AT100" s="40"/>
       <c r="AU100" s="40"/>
@@ -10503,10 +10509,12 @@
       <c r="BY100" s="38"/>
       <c r="BZ100" s="38"/>
     </row>
-    <row r="101" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A101" s="32"/>
       <c r="B101" s="53"/>
-      <c r="C101" s="56"/>
+      <c r="C101" s="56" t="s">
+        <v>124</v>
+      </c>
       <c r="D101" s="54"/>
       <c r="E101" s="35"/>
       <c r="F101" s="35"/>
@@ -10544,10 +10552,10 @@
       <c r="AL101" s="38"/>
       <c r="AM101" s="38"/>
       <c r="AN101" s="38"/>
-      <c r="AO101" s="38"/>
-      <c r="AP101" s="38"/>
-      <c r="AQ101" s="38"/>
-      <c r="AR101" s="40"/>
+      <c r="AO101" s="149"/>
+      <c r="AP101" s="149"/>
+      <c r="AQ101" s="149"/>
+      <c r="AR101" s="147"/>
       <c r="AS101" s="40"/>
       <c r="AT101" s="40"/>
       <c r="AU101" s="40"/>
@@ -10583,10 +10591,12 @@
       <c r="BY101" s="38"/>
       <c r="BZ101" s="38"/>
     </row>
-    <row r="102" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A102" s="32"/>
       <c r="B102" s="53"/>
-      <c r="C102" s="57"/>
+      <c r="C102" s="56" t="s">
+        <v>125</v>
+      </c>
       <c r="D102" s="54"/>
       <c r="E102" s="35"/>
       <c r="F102" s="35"/>
@@ -10624,15 +10634,15 @@
       <c r="AL102" s="38"/>
       <c r="AM102" s="38"/>
       <c r="AN102" s="38"/>
-      <c r="AO102" s="38"/>
-      <c r="AP102" s="38"/>
-      <c r="AQ102" s="38"/>
-      <c r="AR102" s="40"/>
-      <c r="AS102" s="40"/>
-      <c r="AT102" s="40"/>
-      <c r="AU102" s="40"/>
-      <c r="AV102" s="40"/>
-      <c r="AW102" s="38"/>
+      <c r="AO102" s="149"/>
+      <c r="AP102" s="149"/>
+      <c r="AQ102" s="149"/>
+      <c r="AR102" s="149"/>
+      <c r="AS102" s="149"/>
+      <c r="AT102" s="149"/>
+      <c r="AU102" s="149"/>
+      <c r="AV102" s="149"/>
+      <c r="AW102" s="58"/>
       <c r="AX102" s="38"/>
       <c r="AY102" s="38"/>
       <c r="AZ102" s="38"/>
@@ -10663,112 +10673,97 @@
       <c r="BY102" s="38"/>
       <c r="BZ102" s="38"/>
     </row>
-    <row r="103" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="26">
-        <v>4</v>
-      </c>
-      <c r="C103" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="D103" s="28"/>
-      <c r="E103" s="28"/>
-      <c r="F103" s="28"/>
-      <c r="G103" s="28"/>
-      <c r="H103" s="28"/>
-      <c r="I103" s="29"/>
-      <c r="J103" s="30"/>
-      <c r="K103" s="31"/>
-      <c r="L103" s="31"/>
-      <c r="M103" s="29"/>
-      <c r="N103" s="29"/>
-      <c r="O103" s="29"/>
-      <c r="P103" s="29"/>
-      <c r="Q103" s="29"/>
-      <c r="R103" s="29"/>
-      <c r="S103" s="29"/>
-      <c r="T103" s="29"/>
-      <c r="U103" s="29"/>
-      <c r="V103" s="29"/>
-      <c r="W103" s="29"/>
-      <c r="X103" s="29"/>
-      <c r="Y103" s="29"/>
-      <c r="Z103" s="29"/>
-      <c r="AA103" s="29"/>
-      <c r="AB103" s="29"/>
-      <c r="AC103" s="29"/>
-      <c r="AD103" s="29"/>
-      <c r="AE103" s="29"/>
-      <c r="AF103" s="29"/>
-      <c r="AG103" s="29"/>
-      <c r="AH103" s="29"/>
-      <c r="AI103" s="29"/>
-      <c r="AJ103" s="29"/>
-      <c r="AK103" s="29"/>
-      <c r="AL103" s="29"/>
-      <c r="AM103" s="29"/>
-      <c r="AN103" s="29"/>
-      <c r="AO103" s="29"/>
-      <c r="AP103" s="29"/>
-      <c r="AQ103" s="29"/>
-      <c r="AR103" s="29"/>
-      <c r="AS103" s="29"/>
-      <c r="AT103" s="29"/>
-      <c r="AU103" s="29"/>
-      <c r="AV103" s="29"/>
-      <c r="AW103" s="29"/>
-      <c r="AX103" s="29"/>
-      <c r="AY103" s="29"/>
-      <c r="AZ103" s="29"/>
-      <c r="BA103" s="29"/>
-      <c r="BB103" s="29"/>
-      <c r="BC103" s="29"/>
-      <c r="BD103" s="29"/>
-      <c r="BE103" s="29"/>
-      <c r="BF103" s="29"/>
-      <c r="BG103" s="29"/>
-      <c r="BH103" s="29"/>
-      <c r="BI103" s="29"/>
-      <c r="BJ103" s="29"/>
-      <c r="BK103" s="29"/>
-      <c r="BL103" s="29"/>
-      <c r="BM103" s="29"/>
-      <c r="BN103" s="29"/>
-      <c r="BO103" s="29"/>
-      <c r="BP103" s="29"/>
-      <c r="BQ103" s="29"/>
-      <c r="BR103" s="29"/>
-      <c r="BS103" s="29"/>
-      <c r="BT103" s="29"/>
-      <c r="BU103" s="29"/>
-      <c r="BV103" s="29"/>
-      <c r="BW103" s="29"/>
-      <c r="BX103" s="29"/>
-      <c r="BY103" s="29"/>
-      <c r="BZ103" s="29"/>
+    <row r="103" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="32"/>
+      <c r="B103" s="53"/>
+      <c r="C103" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="D103" s="54"/>
+      <c r="E103" s="35"/>
+      <c r="F103" s="35"/>
+      <c r="G103" s="36"/>
+      <c r="H103" s="37"/>
+      <c r="I103" s="42"/>
+      <c r="J103" s="43"/>
+      <c r="K103" s="38"/>
+      <c r="L103" s="38"/>
+      <c r="M103" s="38"/>
+      <c r="N103" s="44"/>
+      <c r="O103" s="44"/>
+      <c r="P103" s="44"/>
+      <c r="Q103" s="44"/>
+      <c r="R103" s="44"/>
+      <c r="S103" s="38"/>
+      <c r="T103" s="38"/>
+      <c r="U103" s="38"/>
+      <c r="V103" s="38"/>
+      <c r="W103" s="38"/>
+      <c r="X103" s="38"/>
+      <c r="Y103" s="38"/>
+      <c r="Z103" s="38"/>
+      <c r="AA103" s="38"/>
+      <c r="AB103" s="38"/>
+      <c r="AC103" s="39"/>
+      <c r="AD103" s="39"/>
+      <c r="AE103" s="39"/>
+      <c r="AF103" s="39"/>
+      <c r="AG103" s="39"/>
+      <c r="AH103" s="38"/>
+      <c r="AI103" s="38"/>
+      <c r="AJ103" s="38"/>
+      <c r="AK103" s="38"/>
+      <c r="AL103" s="38"/>
+      <c r="AM103" s="38"/>
+      <c r="AN103" s="38"/>
+      <c r="AO103" s="124"/>
+      <c r="AP103" s="124"/>
+      <c r="AQ103" s="150"/>
+      <c r="AR103" s="147"/>
+      <c r="AS103" s="40"/>
+      <c r="AT103" s="40"/>
+      <c r="AU103" s="40"/>
+      <c r="AV103" s="40"/>
+      <c r="AW103" s="38"/>
+      <c r="AX103" s="38"/>
+      <c r="AY103" s="38"/>
+      <c r="AZ103" s="38"/>
+      <c r="BA103" s="38"/>
+      <c r="BB103" s="38"/>
+      <c r="BC103" s="38"/>
+      <c r="BD103" s="38"/>
+      <c r="BE103" s="38"/>
+      <c r="BF103" s="38"/>
+      <c r="BG103" s="41"/>
+      <c r="BH103" s="41"/>
+      <c r="BI103" s="41"/>
+      <c r="BJ103" s="41"/>
+      <c r="BK103" s="41"/>
+      <c r="BL103" s="38"/>
+      <c r="BM103" s="38"/>
+      <c r="BN103" s="38"/>
+      <c r="BO103" s="38"/>
+      <c r="BP103" s="38"/>
+      <c r="BQ103" s="38"/>
+      <c r="BR103" s="38"/>
+      <c r="BS103" s="38"/>
+      <c r="BT103" s="38"/>
+      <c r="BU103" s="38"/>
+      <c r="BV103" s="38"/>
+      <c r="BW103" s="38"/>
+      <c r="BX103" s="38"/>
+      <c r="BY103" s="38"/>
+      <c r="BZ103" s="38"/>
     </row>
-    <row r="104" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="33">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C104" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="D104" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E104" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F104" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="G104" s="36" t="e">
-        <f>DAYS360(E104,F104)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H104" s="37">
-        <v>1</v>
-      </c>
+    <row r="104" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="32"/>
+      <c r="B104" s="53"/>
+      <c r="C104" s="56"/>
+      <c r="D104" s="54"/>
+      <c r="E104" s="35"/>
+      <c r="F104" s="35"/>
+      <c r="G104" s="36"/>
+      <c r="H104" s="37"/>
       <c r="I104" s="42"/>
       <c r="J104" s="43"/>
       <c r="K104" s="38"/>
@@ -10840,28 +10835,15 @@
       <c r="BY104" s="38"/>
       <c r="BZ104" s="38"/>
     </row>
-    <row r="105" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="33">
-        <v>4.2</v>
-      </c>
-      <c r="C105" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="D105" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E105" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F105" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="G105" s="36">
-        <v>0</v>
-      </c>
-      <c r="H105" s="37">
-        <v>1</v>
-      </c>
+    <row r="105" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="32"/>
+      <c r="B105" s="53"/>
+      <c r="C105" s="57"/>
+      <c r="D105" s="54"/>
+      <c r="E105" s="35"/>
+      <c r="F105" s="35"/>
+      <c r="G105" s="36"/>
+      <c r="H105" s="37"/>
       <c r="I105" s="42"/>
       <c r="J105" s="43"/>
       <c r="K105" s="38"/>
@@ -10933,121 +10915,110 @@
       <c r="BY105" s="38"/>
       <c r="BZ105" s="38"/>
     </row>
-    <row r="106" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C106" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D106" s="34" t="s">
+    <row r="106" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B106" s="26">
+        <v>4</v>
+      </c>
+      <c r="C106" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="D106" s="28"/>
+      <c r="E106" s="28"/>
+      <c r="F106" s="28"/>
+      <c r="G106" s="28"/>
+      <c r="H106" s="28"/>
+      <c r="I106" s="29"/>
+      <c r="J106" s="30"/>
+      <c r="K106" s="31"/>
+      <c r="L106" s="31"/>
+      <c r="M106" s="29"/>
+      <c r="N106" s="29"/>
+      <c r="O106" s="29"/>
+      <c r="P106" s="29"/>
+      <c r="Q106" s="29"/>
+      <c r="R106" s="29"/>
+      <c r="S106" s="29"/>
+      <c r="T106" s="29"/>
+      <c r="U106" s="29"/>
+      <c r="V106" s="29"/>
+      <c r="W106" s="29"/>
+      <c r="X106" s="29"/>
+      <c r="Y106" s="29"/>
+      <c r="Z106" s="29"/>
+      <c r="AA106" s="29"/>
+      <c r="AB106" s="29"/>
+      <c r="AC106" s="29"/>
+      <c r="AD106" s="29"/>
+      <c r="AE106" s="29"/>
+      <c r="AF106" s="29"/>
+      <c r="AG106" s="29"/>
+      <c r="AH106" s="29"/>
+      <c r="AI106" s="29"/>
+      <c r="AJ106" s="29"/>
+      <c r="AK106" s="29"/>
+      <c r="AL106" s="29"/>
+      <c r="AM106" s="29"/>
+      <c r="AN106" s="29"/>
+      <c r="AO106" s="29"/>
+      <c r="AP106" s="29"/>
+      <c r="AQ106" s="29"/>
+      <c r="AR106" s="29"/>
+      <c r="AS106" s="29"/>
+      <c r="AT106" s="29"/>
+      <c r="AU106" s="29"/>
+      <c r="AV106" s="29"/>
+      <c r="AW106" s="29"/>
+      <c r="AX106" s="29"/>
+      <c r="AY106" s="29"/>
+      <c r="AZ106" s="29"/>
+      <c r="BA106" s="29"/>
+      <c r="BB106" s="29"/>
+      <c r="BC106" s="29"/>
+      <c r="BD106" s="29"/>
+      <c r="BE106" s="29"/>
+      <c r="BF106" s="29"/>
+      <c r="BG106" s="29"/>
+      <c r="BH106" s="29"/>
+      <c r="BI106" s="29"/>
+      <c r="BJ106" s="29"/>
+      <c r="BK106" s="29"/>
+      <c r="BL106" s="29"/>
+      <c r="BM106" s="29"/>
+      <c r="BN106" s="29"/>
+      <c r="BO106" s="29"/>
+      <c r="BP106" s="29"/>
+      <c r="BQ106" s="29"/>
+      <c r="BR106" s="29"/>
+      <c r="BS106" s="29"/>
+      <c r="BT106" s="29"/>
+      <c r="BU106" s="29"/>
+      <c r="BV106" s="29"/>
+      <c r="BW106" s="29"/>
+      <c r="BX106" s="29"/>
+      <c r="BY106" s="29"/>
+      <c r="BZ106" s="29"/>
+    </row>
+    <row r="107" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B107" s="33">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C107" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="D107" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="E106" s="35">
-        <v>44823</v>
-      </c>
-      <c r="F106" s="35">
-        <v>44823</v>
-      </c>
-      <c r="G106" s="36">
-        <f t="shared" ref="G106:G110" si="4">DAYS360(E106,F106)</f>
-        <v>0</v>
-      </c>
-      <c r="H106" s="37">
-        <v>1</v>
-      </c>
-      <c r="I106" s="42"/>
-      <c r="J106" s="43"/>
-      <c r="K106" s="38"/>
-      <c r="L106" s="38"/>
-      <c r="M106" s="38"/>
-      <c r="N106" s="44"/>
-      <c r="O106" s="44"/>
-      <c r="P106" s="44"/>
-      <c r="Q106" s="44"/>
-      <c r="R106" s="44"/>
-      <c r="S106" s="38"/>
-      <c r="T106" s="38"/>
-      <c r="U106" s="38"/>
-      <c r="V106" s="38"/>
-      <c r="W106" s="38"/>
-      <c r="X106" s="38"/>
-      <c r="Y106" s="38"/>
-      <c r="Z106" s="38"/>
-      <c r="AA106" s="38"/>
-      <c r="AB106" s="38"/>
-      <c r="AC106" s="39"/>
-      <c r="AD106" s="39"/>
-      <c r="AE106" s="39"/>
-      <c r="AF106" s="39"/>
-      <c r="AG106" s="39"/>
-      <c r="AH106" s="38"/>
-      <c r="AI106" s="38"/>
-      <c r="AJ106" s="38"/>
-      <c r="AK106" s="38"/>
-      <c r="AL106" s="38"/>
-      <c r="AM106" s="38"/>
-      <c r="AN106" s="38"/>
-      <c r="AO106" s="38"/>
-      <c r="AP106" s="38"/>
-      <c r="AQ106" s="38"/>
-      <c r="AR106" s="40"/>
-      <c r="AS106" s="40"/>
-      <c r="AT106" s="40"/>
-      <c r="AU106" s="40"/>
-      <c r="AV106" s="40"/>
-      <c r="AW106" s="38"/>
-      <c r="AX106" s="38"/>
-      <c r="AY106" s="38"/>
-      <c r="AZ106" s="38"/>
-      <c r="BA106" s="38"/>
-      <c r="BB106" s="38"/>
-      <c r="BC106" s="38"/>
-      <c r="BD106" s="38"/>
-      <c r="BE106" s="38"/>
-      <c r="BF106" s="38"/>
-      <c r="BG106" s="41"/>
-      <c r="BH106" s="41"/>
-      <c r="BI106" s="41"/>
-      <c r="BJ106" s="41"/>
-      <c r="BK106" s="41"/>
-      <c r="BL106" s="38"/>
-      <c r="BM106" s="38"/>
-      <c r="BN106" s="38"/>
-      <c r="BO106" s="38"/>
-      <c r="BP106" s="38"/>
-      <c r="BQ106" s="38"/>
-      <c r="BR106" s="38"/>
-      <c r="BS106" s="38"/>
-      <c r="BT106" s="38"/>
-      <c r="BU106" s="38"/>
-      <c r="BV106" s="38"/>
-      <c r="BW106" s="38"/>
-      <c r="BX106" s="38"/>
-      <c r="BY106" s="38"/>
-      <c r="BZ106" s="38"/>
-    </row>
-    <row r="107" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C107" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="D107" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="E107" s="35">
-        <v>44829</v>
-      </c>
-      <c r="F107" s="35">
-        <v>44829</v>
-      </c>
-      <c r="G107" s="36">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H107" s="52">
+      <c r="E107" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F107" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G107" s="36" t="e">
+        <f>DAYS360(E107,F107)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H107" s="37">
         <v>1</v>
       </c>
       <c r="I107" s="42"/>
@@ -11121,24 +11092,23 @@
       <c r="BY107" s="38"/>
       <c r="BZ107" s="38"/>
     </row>
-    <row r="108" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="33" t="s">
-        <v>48</v>
+    <row r="108" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B108" s="33">
+        <v>4.2</v>
       </c>
       <c r="C108" s="47" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D108" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="E108" s="35">
-        <v>44830</v>
-      </c>
-      <c r="F108" s="35">
-        <v>44830</v>
+      <c r="E108" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F108" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="G108" s="36">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H108" s="37">
@@ -11215,24 +11185,24 @@
       <c r="BY108" s="38"/>
       <c r="BZ108" s="38"/>
     </row>
-    <row r="109" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B109" s="33" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C109" s="47" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D109" s="34" t="s">
         <v>18</v>
       </c>
       <c r="E109" s="35">
-        <v>44837</v>
+        <v>44823</v>
       </c>
       <c r="F109" s="35">
-        <v>44837</v>
+        <v>44823</v>
       </c>
       <c r="G109" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G109:G113" si="4">DAYS360(E109,F109)</f>
         <v>0</v>
       </c>
       <c r="H109" s="37">
@@ -11309,25 +11279,27 @@
       <c r="BY109" s="38"/>
       <c r="BZ109" s="38"/>
     </row>
-    <row r="110" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="33"/>
+    <row r="110" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B110" s="33" t="s">
+        <v>49</v>
+      </c>
       <c r="C110" s="47" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D110" s="34" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E110" s="35">
-        <v>44844</v>
+        <v>44829</v>
       </c>
       <c r="F110" s="35">
-        <v>44844</v>
+        <v>44829</v>
       </c>
       <c r="G110" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H110" s="37">
+      <c r="H110" s="52">
         <v>1</v>
       </c>
       <c r="I110" s="42"/>
@@ -11401,24 +11373,24 @@
       <c r="BY110" s="38"/>
       <c r="BZ110" s="38"/>
     </row>
-    <row r="111" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B111" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C111" s="106" t="s">
-        <v>92</v>
+        <v>48</v>
+      </c>
+      <c r="C111" s="47" t="s">
+        <v>61</v>
       </c>
       <c r="D111" s="34" t="s">
         <v>18</v>
       </c>
       <c r="E111" s="35">
-        <v>44844</v>
+        <v>44830</v>
       </c>
       <c r="F111" s="35">
-        <v>44844</v>
+        <v>44830</v>
       </c>
       <c r="G111" s="36">
-        <f t="shared" ref="G111" si="5">DAYS360(E111,F111)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H111" s="37">
@@ -11495,107 +11467,367 @@
       <c r="BY111" s="38"/>
       <c r="BZ111" s="38"/>
     </row>
-    <row r="112" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="107"/>
-      <c r="C112" s="108"/>
-      <c r="D112" s="109"/>
-      <c r="E112" s="110"/>
-      <c r="F112" s="110"/>
-      <c r="G112" s="111"/>
-      <c r="H112" s="112"/>
-      <c r="I112" s="113"/>
-      <c r="J112" s="114"/>
-      <c r="K112" s="115"/>
-      <c r="L112" s="115"/>
-      <c r="M112" s="115"/>
-      <c r="N112" s="116"/>
-      <c r="O112" s="116"/>
-      <c r="P112" s="116"/>
-      <c r="Q112" s="116"/>
-      <c r="R112" s="116"/>
-      <c r="S112" s="115"/>
-      <c r="T112" s="115"/>
-      <c r="U112" s="115"/>
-      <c r="V112" s="115"/>
-      <c r="W112" s="115"/>
-      <c r="X112" s="115"/>
-      <c r="Y112" s="115"/>
-      <c r="Z112" s="115"/>
-      <c r="AA112" s="115"/>
-      <c r="AB112" s="115"/>
-      <c r="AC112" s="117"/>
-      <c r="AD112" s="117"/>
-      <c r="AE112" s="117"/>
-      <c r="AF112" s="117"/>
-      <c r="AG112" s="117"/>
-      <c r="AH112" s="115"/>
-      <c r="AI112" s="115"/>
-      <c r="AJ112" s="115"/>
-      <c r="AK112" s="115"/>
-      <c r="AL112" s="115"/>
-      <c r="AM112" s="115"/>
-      <c r="AN112" s="115"/>
-      <c r="AO112" s="115"/>
-      <c r="AP112" s="115"/>
-      <c r="AQ112" s="115"/>
-      <c r="AR112" s="118"/>
-      <c r="AS112" s="118"/>
-      <c r="AT112" s="118"/>
-      <c r="AU112" s="118"/>
-      <c r="AV112" s="118"/>
-      <c r="AW112" s="115"/>
-      <c r="AX112" s="115"/>
-      <c r="AY112" s="115"/>
-      <c r="AZ112" s="115"/>
-      <c r="BA112" s="115"/>
-      <c r="BB112" s="115"/>
-      <c r="BC112" s="115"/>
-      <c r="BD112" s="115"/>
-      <c r="BE112" s="115"/>
-      <c r="BF112" s="115"/>
-      <c r="BG112" s="119"/>
-      <c r="BH112" s="119"/>
-      <c r="BI112" s="119"/>
-      <c r="BJ112" s="119"/>
-      <c r="BK112" s="119"/>
-      <c r="BL112" s="115"/>
-      <c r="BM112" s="115"/>
-      <c r="BN112" s="115"/>
-      <c r="BO112" s="115"/>
-      <c r="BP112" s="115"/>
-      <c r="BQ112" s="115"/>
-      <c r="BR112" s="115"/>
-      <c r="BS112" s="115"/>
-      <c r="BT112" s="115"/>
-      <c r="BU112" s="115"/>
-      <c r="BV112" s="115"/>
-      <c r="BW112" s="115"/>
-      <c r="BX112" s="115"/>
-      <c r="BY112" s="115"/>
-      <c r="BZ112" s="115"/>
+    <row r="112" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B112" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C112" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D112" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E112" s="35">
+        <v>44837</v>
+      </c>
+      <c r="F112" s="35">
+        <v>44837</v>
+      </c>
+      <c r="G112" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H112" s="37">
+        <v>1</v>
+      </c>
+      <c r="I112" s="42"/>
+      <c r="J112" s="43"/>
+      <c r="K112" s="38"/>
+      <c r="L112" s="38"/>
+      <c r="M112" s="38"/>
+      <c r="N112" s="44"/>
+      <c r="O112" s="44"/>
+      <c r="P112" s="44"/>
+      <c r="Q112" s="44"/>
+      <c r="R112" s="44"/>
+      <c r="S112" s="38"/>
+      <c r="T112" s="38"/>
+      <c r="U112" s="38"/>
+      <c r="V112" s="38"/>
+      <c r="W112" s="38"/>
+      <c r="X112" s="38"/>
+      <c r="Y112" s="38"/>
+      <c r="Z112" s="38"/>
+      <c r="AA112" s="38"/>
+      <c r="AB112" s="38"/>
+      <c r="AC112" s="39"/>
+      <c r="AD112" s="39"/>
+      <c r="AE112" s="39"/>
+      <c r="AF112" s="39"/>
+      <c r="AG112" s="39"/>
+      <c r="AH112" s="38"/>
+      <c r="AI112" s="38"/>
+      <c r="AJ112" s="38"/>
+      <c r="AK112" s="38"/>
+      <c r="AL112" s="38"/>
+      <c r="AM112" s="38"/>
+      <c r="AN112" s="38"/>
+      <c r="AO112" s="38"/>
+      <c r="AP112" s="38"/>
+      <c r="AQ112" s="38"/>
+      <c r="AR112" s="40"/>
+      <c r="AS112" s="40"/>
+      <c r="AT112" s="40"/>
+      <c r="AU112" s="40"/>
+      <c r="AV112" s="40"/>
+      <c r="AW112" s="38"/>
+      <c r="AX112" s="38"/>
+      <c r="AY112" s="38"/>
+      <c r="AZ112" s="38"/>
+      <c r="BA112" s="38"/>
+      <c r="BB112" s="38"/>
+      <c r="BC112" s="38"/>
+      <c r="BD112" s="38"/>
+      <c r="BE112" s="38"/>
+      <c r="BF112" s="38"/>
+      <c r="BG112" s="41"/>
+      <c r="BH112" s="41"/>
+      <c r="BI112" s="41"/>
+      <c r="BJ112" s="41"/>
+      <c r="BK112" s="41"/>
+      <c r="BL112" s="38"/>
+      <c r="BM112" s="38"/>
+      <c r="BN112" s="38"/>
+      <c r="BO112" s="38"/>
+      <c r="BP112" s="38"/>
+      <c r="BQ112" s="38"/>
+      <c r="BR112" s="38"/>
+      <c r="BS112" s="38"/>
+      <c r="BT112" s="38"/>
+      <c r="BU112" s="38"/>
+      <c r="BV112" s="38"/>
+      <c r="BW112" s="38"/>
+      <c r="BX112" s="38"/>
+      <c r="BY112" s="38"/>
+      <c r="BZ112" s="38"/>
+    </row>
+    <row r="113" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B113" s="33"/>
+      <c r="C113" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D113" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E113" s="35">
+        <v>44844</v>
+      </c>
+      <c r="F113" s="35">
+        <v>44844</v>
+      </c>
+      <c r="G113" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H113" s="37">
+        <v>1</v>
+      </c>
+      <c r="I113" s="42"/>
+      <c r="J113" s="43"/>
+      <c r="K113" s="38"/>
+      <c r="L113" s="38"/>
+      <c r="M113" s="38"/>
+      <c r="N113" s="44"/>
+      <c r="O113" s="44"/>
+      <c r="P113" s="44"/>
+      <c r="Q113" s="44"/>
+      <c r="R113" s="44"/>
+      <c r="S113" s="38"/>
+      <c r="T113" s="38"/>
+      <c r="U113" s="38"/>
+      <c r="V113" s="38"/>
+      <c r="W113" s="38"/>
+      <c r="X113" s="38"/>
+      <c r="Y113" s="38"/>
+      <c r="Z113" s="38"/>
+      <c r="AA113" s="38"/>
+      <c r="AB113" s="38"/>
+      <c r="AC113" s="39"/>
+      <c r="AD113" s="39"/>
+      <c r="AE113" s="39"/>
+      <c r="AF113" s="39"/>
+      <c r="AG113" s="39"/>
+      <c r="AH113" s="38"/>
+      <c r="AI113" s="38"/>
+      <c r="AJ113" s="38"/>
+      <c r="AK113" s="38"/>
+      <c r="AL113" s="38"/>
+      <c r="AM113" s="38"/>
+      <c r="AN113" s="38"/>
+      <c r="AO113" s="38"/>
+      <c r="AP113" s="38"/>
+      <c r="AQ113" s="38"/>
+      <c r="AR113" s="40"/>
+      <c r="AS113" s="40"/>
+      <c r="AT113" s="40"/>
+      <c r="AU113" s="40"/>
+      <c r="AV113" s="40"/>
+      <c r="AW113" s="38"/>
+      <c r="AX113" s="38"/>
+      <c r="AY113" s="38"/>
+      <c r="AZ113" s="38"/>
+      <c r="BA113" s="38"/>
+      <c r="BB113" s="38"/>
+      <c r="BC113" s="38"/>
+      <c r="BD113" s="38"/>
+      <c r="BE113" s="38"/>
+      <c r="BF113" s="38"/>
+      <c r="BG113" s="41"/>
+      <c r="BH113" s="41"/>
+      <c r="BI113" s="41"/>
+      <c r="BJ113" s="41"/>
+      <c r="BK113" s="41"/>
+      <c r="BL113" s="38"/>
+      <c r="BM113" s="38"/>
+      <c r="BN113" s="38"/>
+      <c r="BO113" s="38"/>
+      <c r="BP113" s="38"/>
+      <c r="BQ113" s="38"/>
+      <c r="BR113" s="38"/>
+      <c r="BS113" s="38"/>
+      <c r="BT113" s="38"/>
+      <c r="BU113" s="38"/>
+      <c r="BV113" s="38"/>
+      <c r="BW113" s="38"/>
+      <c r="BX113" s="38"/>
+      <c r="BY113" s="38"/>
+      <c r="BZ113" s="38"/>
+    </row>
+    <row r="114" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B114" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C114" s="106" t="s">
+        <v>92</v>
+      </c>
+      <c r="D114" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E114" s="35">
+        <v>44844</v>
+      </c>
+      <c r="F114" s="35">
+        <v>44844</v>
+      </c>
+      <c r="G114" s="36">
+        <f t="shared" ref="G114" si="5">DAYS360(E114,F114)</f>
+        <v>0</v>
+      </c>
+      <c r="H114" s="37">
+        <v>1</v>
+      </c>
+      <c r="I114" s="42"/>
+      <c r="J114" s="43"/>
+      <c r="K114" s="38"/>
+      <c r="L114" s="38"/>
+      <c r="M114" s="38"/>
+      <c r="N114" s="44"/>
+      <c r="O114" s="44"/>
+      <c r="P114" s="44"/>
+      <c r="Q114" s="44"/>
+      <c r="R114" s="44"/>
+      <c r="S114" s="38"/>
+      <c r="T114" s="38"/>
+      <c r="U114" s="38"/>
+      <c r="V114" s="38"/>
+      <c r="W114" s="38"/>
+      <c r="X114" s="38"/>
+      <c r="Y114" s="38"/>
+      <c r="Z114" s="38"/>
+      <c r="AA114" s="38"/>
+      <c r="AB114" s="38"/>
+      <c r="AC114" s="39"/>
+      <c r="AD114" s="39"/>
+      <c r="AE114" s="39"/>
+      <c r="AF114" s="39"/>
+      <c r="AG114" s="39"/>
+      <c r="AH114" s="38"/>
+      <c r="AI114" s="38"/>
+      <c r="AJ114" s="38"/>
+      <c r="AK114" s="38"/>
+      <c r="AL114" s="38"/>
+      <c r="AM114" s="38"/>
+      <c r="AN114" s="38"/>
+      <c r="AO114" s="38"/>
+      <c r="AP114" s="38"/>
+      <c r="AQ114" s="38"/>
+      <c r="AR114" s="40"/>
+      <c r="AS114" s="40"/>
+      <c r="AT114" s="40"/>
+      <c r="AU114" s="40"/>
+      <c r="AV114" s="40"/>
+      <c r="AW114" s="38"/>
+      <c r="AX114" s="38"/>
+      <c r="AY114" s="38"/>
+      <c r="AZ114" s="38"/>
+      <c r="BA114" s="38"/>
+      <c r="BB114" s="38"/>
+      <c r="BC114" s="38"/>
+      <c r="BD114" s="38"/>
+      <c r="BE114" s="38"/>
+      <c r="BF114" s="38"/>
+      <c r="BG114" s="41"/>
+      <c r="BH114" s="41"/>
+      <c r="BI114" s="41"/>
+      <c r="BJ114" s="41"/>
+      <c r="BK114" s="41"/>
+      <c r="BL114" s="38"/>
+      <c r="BM114" s="38"/>
+      <c r="BN114" s="38"/>
+      <c r="BO114" s="38"/>
+      <c r="BP114" s="38"/>
+      <c r="BQ114" s="38"/>
+      <c r="BR114" s="38"/>
+      <c r="BS114" s="38"/>
+      <c r="BT114" s="38"/>
+      <c r="BU114" s="38"/>
+      <c r="BV114" s="38"/>
+      <c r="BW114" s="38"/>
+      <c r="BX114" s="38"/>
+      <c r="BY114" s="38"/>
+      <c r="BZ114" s="38"/>
+    </row>
+    <row r="115" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B115" s="107"/>
+      <c r="C115" s="108"/>
+      <c r="D115" s="109"/>
+      <c r="E115" s="110"/>
+      <c r="F115" s="110"/>
+      <c r="G115" s="111"/>
+      <c r="H115" s="112"/>
+      <c r="I115" s="113"/>
+      <c r="J115" s="114"/>
+      <c r="K115" s="115"/>
+      <c r="L115" s="115"/>
+      <c r="M115" s="115"/>
+      <c r="N115" s="116"/>
+      <c r="O115" s="116"/>
+      <c r="P115" s="116"/>
+      <c r="Q115" s="116"/>
+      <c r="R115" s="116"/>
+      <c r="S115" s="115"/>
+      <c r="T115" s="115"/>
+      <c r="U115" s="115"/>
+      <c r="V115" s="115"/>
+      <c r="W115" s="115"/>
+      <c r="X115" s="115"/>
+      <c r="Y115" s="115"/>
+      <c r="Z115" s="115"/>
+      <c r="AA115" s="115"/>
+      <c r="AB115" s="115"/>
+      <c r="AC115" s="117"/>
+      <c r="AD115" s="117"/>
+      <c r="AE115" s="117"/>
+      <c r="AF115" s="117"/>
+      <c r="AG115" s="117"/>
+      <c r="AH115" s="115"/>
+      <c r="AI115" s="115"/>
+      <c r="AJ115" s="115"/>
+      <c r="AK115" s="115"/>
+      <c r="AL115" s="115"/>
+      <c r="AM115" s="115"/>
+      <c r="AN115" s="115"/>
+      <c r="AO115" s="115"/>
+      <c r="AP115" s="115"/>
+      <c r="AQ115" s="115"/>
+      <c r="AR115" s="118"/>
+      <c r="AS115" s="118"/>
+      <c r="AT115" s="118"/>
+      <c r="AU115" s="118"/>
+      <c r="AV115" s="118"/>
+      <c r="AW115" s="115"/>
+      <c r="AX115" s="115"/>
+      <c r="AY115" s="115"/>
+      <c r="AZ115" s="115"/>
+      <c r="BA115" s="115"/>
+      <c r="BB115" s="115"/>
+      <c r="BC115" s="115"/>
+      <c r="BD115" s="115"/>
+      <c r="BE115" s="115"/>
+      <c r="BF115" s="115"/>
+      <c r="BG115" s="119"/>
+      <c r="BH115" s="119"/>
+      <c r="BI115" s="119"/>
+      <c r="BJ115" s="119"/>
+      <c r="BK115" s="119"/>
+      <c r="BL115" s="115"/>
+      <c r="BM115" s="115"/>
+      <c r="BN115" s="115"/>
+      <c r="BO115" s="115"/>
+      <c r="BP115" s="115"/>
+      <c r="BQ115" s="115"/>
+      <c r="BR115" s="115"/>
+      <c r="BS115" s="115"/>
+      <c r="BT115" s="115"/>
+      <c r="BU115" s="115"/>
+      <c r="BV115" s="115"/>
+      <c r="BW115" s="115"/>
+      <c r="BX115" s="115"/>
+      <c r="BY115" s="115"/>
+      <c r="BZ115" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:W9"/>
-    <mergeCell ref="X9:AL9"/>
-    <mergeCell ref="AM9:BA9"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="AC10:AG10"/>
-    <mergeCell ref="AH10:AL10"/>
-    <mergeCell ref="AM10:AQ10"/>
-    <mergeCell ref="AR10:AV10"/>
-    <mergeCell ref="AW10:BA10"/>
     <mergeCell ref="BB9:BZ9"/>
     <mergeCell ref="I10:M10"/>
     <mergeCell ref="N10:R10"/>
@@ -11612,9 +11844,29 @@
     <mergeCell ref="BQ10:BU10"/>
     <mergeCell ref="BV10:BZ10"/>
     <mergeCell ref="S10:W10"/>
+    <mergeCell ref="AM9:BA9"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="AC10:AG10"/>
+    <mergeCell ref="AH10:AL10"/>
+    <mergeCell ref="AM10:AQ10"/>
+    <mergeCell ref="AR10:AV10"/>
+    <mergeCell ref="AW10:BA10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:W9"/>
+    <mergeCell ref="X9:AL9"/>
   </mergeCells>
   <phoneticPr fontId="35" type="noConversion"/>
-  <conditionalFormatting sqref="H12:H21 H23:H112">
+  <conditionalFormatting sqref="H12:H21 H23:H115">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -11624,7 +11876,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H21 H23:H112">
+  <conditionalFormatting sqref="H12:H21 H23:H115">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -11649,6 +11901,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7EF2104F2CEFE4DACFBF5BA7D93FB4D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb0ed258f694207805e211ca255f9b46">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6b71f768-6d8b-468c-a986-1e1afc74f0e3" xmlns:ns4="d07d918a-d172-4450-8f4a-7b087689ff85" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c03c9fe975be0719773112499dde791" ns3:_="" ns4:_="">
     <xsd:import namespace="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
@@ -11877,12 +12135,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
@@ -11892,6 +12144,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FABC364-430D-422C-AD85-145699D2125C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11908,21 +12177,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>